<commit_message>
Cambio de F a la izquierda
Cambio de F a la izquierda
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion09/ESCALETAFINAL CN_09_09_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion09/ESCALETAFINAL CN_09_09_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Desktop\Edición Planeta\CN_09_09_CO_UNI\Final CN_09_09_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado09\guion09\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -774,7 +774,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1032,11 +1032,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1117,13 +1143,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1137,6 +1163,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1420,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,8 +1469,8 @@
     <col min="10" max="10" width="92.28515625" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.7109375" style="9" customWidth="1"/>
-    <col min="13" max="13" width="14" style="9" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="14" max="14" width="14" style="9" customWidth="1"/>
     <col min="15" max="15" width="60" style="10" customWidth="1"/>
     <col min="16" max="16" width="21.140625" style="7" customWidth="1"/>
     <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -1449,34 +1481,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="53" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="57" t="s">
@@ -1485,58 +1517,58 @@
       <c r="L1" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="52" t="s">
+      <c r="N1" s="60"/>
+      <c r="O1" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="52" t="s">
+      <c r="P1" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="52" t="s">
+      <c r="R1" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="52" t="s">
+      <c r="S1" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="52" t="s">
+      <c r="T1" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="52" t="s">
+      <c r="U1" s="53" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="12" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="58"/>
       <c r="L2" s="56"/>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="N2" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -1674,10 +1706,10 @@
         <v>69</v>
       </c>
       <c r="L6" s="43"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46" t="s">
+      <c r="M6" s="46" t="s">
         <v>34</v>
       </c>
+      <c r="N6" s="46"/>
       <c r="O6" s="45" t="s">
         <v>119</v>
       </c>
@@ -1792,10 +1824,10 @@
       <c r="L8" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="46" t="s">
+      <c r="M8" s="46"/>
+      <c r="N8" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="N8" s="46"/>
       <c r="O8" s="45"/>
       <c r="P8" s="44" t="s">
         <v>19</v>
@@ -1851,10 +1883,10 @@
       <c r="L9" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="46" t="s">
+      <c r="M9" s="46"/>
+      <c r="N9" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N9" s="46"/>
       <c r="O9" s="45"/>
       <c r="P9" s="44" t="s">
         <v>20</v>
@@ -1910,10 +1942,10 @@
       <c r="L10" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="46" t="s">
+      <c r="M10" s="46"/>
+      <c r="N10" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="N10" s="46"/>
       <c r="O10" s="45"/>
       <c r="P10" s="44" t="s">
         <v>20</v>
@@ -1969,10 +2001,10 @@
       <c r="L11" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M11" s="46" t="s">
+      <c r="M11" s="46"/>
+      <c r="N11" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="N11" s="46"/>
       <c r="O11" s="45"/>
       <c r="P11" s="44" t="s">
         <v>19</v>
@@ -2030,10 +2062,10 @@
       <c r="L12" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M12" s="46" t="s">
+      <c r="M12" s="46"/>
+      <c r="N12" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="N12" s="46"/>
       <c r="O12" s="45"/>
       <c r="P12" s="44" t="s">
         <v>19</v>
@@ -2091,10 +2123,10 @@
       <c r="L13" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M13" s="46" t="s">
+      <c r="M13" s="46"/>
+      <c r="N13" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="N13" s="46"/>
       <c r="O13" s="45"/>
       <c r="P13" s="44" t="s">
         <v>19</v>
@@ -2152,10 +2184,10 @@
       <c r="L14" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M14" s="46" t="s">
+      <c r="M14" s="46"/>
+      <c r="N14" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N14" s="46"/>
       <c r="O14" s="45"/>
       <c r="P14" s="44" t="s">
         <v>19</v>
@@ -2216,10 +2248,10 @@
       <c r="L15" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M15" s="46" t="s">
+      <c r="M15" s="46"/>
+      <c r="N15" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="N15" s="46"/>
       <c r="O15" s="45"/>
       <c r="P15" s="44" t="s">
         <v>19</v>
@@ -2277,10 +2309,10 @@
       <c r="L16" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M16" s="46" t="s">
+      <c r="M16" s="46"/>
+      <c r="N16" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="46"/>
       <c r="O16" s="45"/>
       <c r="P16" s="44" t="s">
         <v>20</v>
@@ -2338,10 +2370,10 @@
       <c r="L17" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46" t="s">
+      <c r="M17" s="46" t="s">
         <v>36</v>
       </c>
+      <c r="N17" s="46"/>
       <c r="O17" s="45"/>
       <c r="P17" s="44" t="s">
         <v>19</v>
@@ -2458,10 +2490,10 @@
       <c r="L19" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M19" s="46" t="s">
+      <c r="M19" s="46"/>
+      <c r="N19" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="N19" s="46"/>
       <c r="O19" s="45"/>
       <c r="P19" s="44" t="s">
         <v>19</v>
@@ -2519,10 +2551,10 @@
       <c r="L20" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M20" s="46" t="s">
+      <c r="M20" s="46"/>
+      <c r="N20" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="N20" s="46"/>
       <c r="O20" s="45"/>
       <c r="P20" s="44" t="s">
         <v>19</v>
@@ -2580,10 +2612,10 @@
       <c r="L21" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M21" s="46" t="s">
+      <c r="M21" s="46"/>
+      <c r="N21" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="N21" s="46"/>
       <c r="O21" s="45"/>
       <c r="P21" s="44" t="s">
         <v>19</v>
@@ -2641,10 +2673,10 @@
       <c r="L22" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M22" s="46" t="s">
+      <c r="M22" s="46"/>
+      <c r="N22" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="N22" s="46"/>
       <c r="O22" s="45"/>
       <c r="P22" s="44" t="s">
         <v>19</v>
@@ -2702,10 +2734,10 @@
       <c r="L23" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="46" t="s">
+      <c r="M23" s="46"/>
+      <c r="N23" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N23" s="46"/>
       <c r="O23" s="45"/>
       <c r="P23" s="44" t="s">
         <v>20</v>
@@ -2763,10 +2795,10 @@
       <c r="L24" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46" t="s">
+      <c r="M24" s="46" t="s">
         <v>36</v>
       </c>
+      <c r="N24" s="46"/>
       <c r="O24" s="45"/>
       <c r="P24" s="44" t="s">
         <v>19</v>
@@ -2822,10 +2854,10 @@
       <c r="L25" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M25" s="46" t="s">
+      <c r="M25" s="46"/>
+      <c r="N25" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N25" s="46"/>
       <c r="O25" s="45"/>
       <c r="P25" s="44" t="s">
         <v>19</v>
@@ -2881,10 +2913,10 @@
       <c r="L26" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M26" s="46" t="s">
+      <c r="M26" s="46"/>
+      <c r="N26" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="N26" s="46"/>
       <c r="O26" s="45"/>
       <c r="P26" s="44" t="s">
         <v>19</v>
@@ -3039,10 +3071,10 @@
       <c r="L30" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="M30" s="46"/>
-      <c r="N30" s="46" t="s">
+      <c r="M30" s="46" t="s">
         <v>44</v>
       </c>
+      <c r="N30" s="46"/>
       <c r="O30" s="45"/>
       <c r="P30" s="44" t="s">
         <v>19</v>
@@ -3098,10 +3130,10 @@
       <c r="L31" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M31" s="46" t="s">
+      <c r="M31" s="46"/>
+      <c r="N31" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="N31" s="46"/>
       <c r="O31" s="45"/>
       <c r="P31" s="44" t="s">
         <v>19</v>
@@ -3155,10 +3187,10 @@
       <c r="L32" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M32" s="46" t="s">
+      <c r="M32" s="46"/>
+      <c r="N32" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="N32" s="46"/>
       <c r="O32" s="45"/>
       <c r="P32" s="44" t="s">
         <v>19</v>
@@ -3212,10 +3244,10 @@
       <c r="L33" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M33" s="46" t="s">
+      <c r="M33" s="46"/>
+      <c r="N33" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="N33" s="46"/>
       <c r="O33" s="45"/>
       <c r="P33" s="44" t="s">
         <v>19</v>
@@ -3269,10 +3301,10 @@
       <c r="L34" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M34" s="46" t="s">
+      <c r="M34" s="46"/>
+      <c r="N34" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="N34" s="46"/>
       <c r="O34" s="45"/>
       <c r="P34" s="44" t="s">
         <v>19</v>
@@ -3371,10 +3403,10 @@
       <c r="L36" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M36" s="46" t="s">
+      <c r="M36" s="46"/>
+      <c r="N36" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N36" s="46"/>
       <c r="O36" s="45"/>
       <c r="P36" s="44" t="s">
         <v>20</v>
@@ -3426,10 +3458,10 @@
       <c r="L37" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="M37" s="46" t="s">
+      <c r="M37" s="46"/>
+      <c r="N37" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="N37" s="46"/>
       <c r="O37" s="45"/>
       <c r="P37" s="44" t="s">
         <v>20</v>
@@ -4877,13 +4909,14 @@
       <c r="U99" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U36">
-    <filterColumn colId="12" showButton="0"/>
-  </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="M1:N1"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="S1:S2"/>
@@ -4896,11 +4929,7 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4935,13 +4964,13 @@
           <x14:formula1>
             <xm:f>DATOS!$C$2:$C$39</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M99</xm:sqref>
+          <xm:sqref>N3:N99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$2:$B$14</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N99</xm:sqref>
+          <xm:sqref>M3:M99</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Complementar campo de fichas
Complementar campo de fichas
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion09/ESCALETAFINAL CN_09_09_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion09/ESCALETAFINAL CN_09_09_CO.xlsx
@@ -1452,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2723,7 +2723,7 @@
         <v>18</v>
       </c>
       <c r="I23" s="37" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J23" s="50" t="s">
         <v>202</v>
@@ -4910,11 +4910,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="U1:U2"/>
@@ -4930,6 +4925,11 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambio en título y descripción de un recurso
Cambio en título y descripción de un recurso
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion09/ESCALETAFINAL CN_09_09_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion09/ESCALETAFINAL CN_09_09_CO.xlsx
@@ -16,7 +16,7 @@
     <sheet name="DATOS" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$U$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$U$37</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="216">
   <si>
     <t>Asignatura</t>
   </si>
@@ -384,12 +384,6 @@
     <t xml:space="preserve">Competencias </t>
   </si>
   <si>
-    <t>La solvatación</t>
-  </si>
-  <si>
-    <t>Secuencia de imágenes que permite explicar el proceso de solvatación</t>
-  </si>
-  <si>
     <t>Secuencia de imágenes</t>
   </si>
   <si>
@@ -682,6 +676,9 @@
   </si>
   <si>
     <t>Actividad que permite ejercitar  los cálculos de la concentración de disoluciones en porcentaje en partes por millón</t>
+  </si>
+  <si>
+    <t>Secuencia de imágenes que permite explicar las caracteristicas de las disoluciones y el proceso de disolución</t>
   </si>
 </sst>
 </file>
@@ -1450,10 +1447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W99"/>
+  <dimension ref="A1:W100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,9 +1580,7 @@
       <c r="D3" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="47" t="s">
-        <v>93</v>
-      </c>
+      <c r="E3" s="47"/>
       <c r="F3" s="28"/>
       <c r="G3" s="33"/>
       <c r="H3" s="34"/>
@@ -1603,7 +1598,7 @@
       <c r="T3" s="14"/>
       <c r="U3" s="4"/>
     </row>
-    <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>67</v>
       </c>
@@ -1616,29 +1611,53 @@
       <c r="D4" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="F4" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="42"/>
+      <c r="E4" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="28"/>
+      <c r="G4" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="37">
+        <v>1</v>
+      </c>
+      <c r="I4" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="K4" s="42" t="s">
+        <v>69</v>
+      </c>
       <c r="L4" s="43"/>
-      <c r="M4" s="46"/>
+      <c r="M4" s="46" t="s">
+        <v>34</v>
+      </c>
       <c r="N4" s="46"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="2"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="O4" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="P4" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>6</v>
+      </c>
+      <c r="R4" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>67</v>
       </c>
@@ -1654,10 +1673,10 @@
       <c r="E5" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="F5" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" s="51"/>
+      <c r="F5" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="36"/>
       <c r="H5" s="37"/>
       <c r="I5" s="37"/>
       <c r="J5" s="38"/>
@@ -1687,50 +1706,26 @@
         <v>92</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="F6" s="30"/>
-      <c r="G6" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="H6" s="37">
-        <v>1</v>
-      </c>
-      <c r="I6" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="K6" s="42" t="s">
-        <v>69</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="F6" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="51"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="42"/>
       <c r="L6" s="43"/>
-      <c r="M6" s="46" t="s">
-        <v>34</v>
-      </c>
+      <c r="M6" s="46"/>
       <c r="N6" s="46"/>
-      <c r="O6" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="P6" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>6</v>
-      </c>
-      <c r="R6" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="S6" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="T6" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>123</v>
-      </c>
+      <c r="O6" s="45"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="2"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
@@ -1746,48 +1741,24 @@
         <v>92</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F7" s="30"/>
-      <c r="G7" s="36" t="s">
-        <v>98</v>
-      </c>
-      <c r="H7" s="37">
-        <v>2</v>
-      </c>
-      <c r="I7" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="K7" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="L7" s="43" t="s">
-        <v>31</v>
-      </c>
+      <c r="G7" s="36"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="43"/>
       <c r="M7" s="46"/>
       <c r="N7" s="46"/>
       <c r="O7" s="45"/>
-      <c r="P7" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="R7" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="S7" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="T7" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>129</v>
-      </c>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="2"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
@@ -1807,45 +1778,43 @@
       </c>
       <c r="F8" s="30"/>
       <c r="G8" s="36" t="s">
-        <v>165</v>
+        <v>98</v>
       </c>
       <c r="H8" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I8" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" s="38" t="s">
-        <v>166</v>
+        <v>122</v>
       </c>
       <c r="K8" s="42" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L8" s="43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M8" s="46"/>
-      <c r="N8" s="46" t="s">
-        <v>24</v>
-      </c>
+      <c r="N8" s="46"/>
       <c r="O8" s="45"/>
       <c r="P8" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="1">
-        <v>6</v>
+      <c r="Q8" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="R8" s="13" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="S8" s="13" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="T8" s="13" t="s">
-        <v>167</v>
+        <v>126</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -1862,49 +1831,49 @@
         <v>92</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9" s="30"/>
       <c r="G9" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H9" s="37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I9" s="37" t="s">
         <v>20</v>
       </c>
       <c r="J9" s="38" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="K9" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L9" s="43" t="s">
         <v>32</v>
       </c>
       <c r="M9" s="46"/>
       <c r="N9" s="46" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O9" s="45"/>
       <c r="P9" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>125</v>
+        <v>19</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>6</v>
       </c>
       <c r="R9" s="13" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="S9" s="13" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="T9" s="13" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -1924,46 +1893,46 @@
         <v>99</v>
       </c>
       <c r="F10" s="30"/>
-      <c r="G10" s="51" t="s">
-        <v>163</v>
+      <c r="G10" s="36" t="s">
+        <v>166</v>
       </c>
       <c r="H10" s="37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I10" s="37" t="s">
         <v>20</v>
       </c>
       <c r="J10" s="38" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="K10" s="42" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L10" s="43" t="s">
         <v>32</v>
       </c>
       <c r="M10" s="46"/>
       <c r="N10" s="46" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="O10" s="45"/>
       <c r="P10" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="1">
-        <v>6</v>
+      <c r="Q10" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="R10" s="13" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="S10" s="13" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="T10" s="13" t="s">
-        <v>214</v>
+        <v>168</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -1979,21 +1948,21 @@
       <c r="D11" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="E11" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="36" t="s">
-        <v>141</v>
+      <c r="E11" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="30"/>
+      <c r="G11" s="51" t="s">
+        <v>161</v>
       </c>
       <c r="H11" s="37">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I11" s="37" t="s">
         <v>20</v>
       </c>
       <c r="J11" s="38" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="K11" s="42" t="s">
         <v>69</v>
@@ -2003,29 +1972,29 @@
       </c>
       <c r="M11" s="46"/>
       <c r="N11" s="46" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="O11" s="45"/>
       <c r="P11" s="44" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q11" s="1">
         <v>6</v>
       </c>
       <c r="R11" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S11" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T11" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="U11" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="T11" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>67</v>
       </c>
@@ -2035,26 +2004,24 @@
       <c r="C12" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>103</v>
-      </c>
+      <c r="D12" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="F12" s="28"/>
       <c r="G12" s="36" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
       <c r="H12" s="37">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I12" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="50" t="s">
-        <v>175</v>
+      <c r="J12" s="38" t="s">
+        <v>140</v>
       </c>
       <c r="K12" s="42" t="s">
         <v>69</v>
@@ -2064,7 +2031,7 @@
       </c>
       <c r="M12" s="46"/>
       <c r="N12" s="46" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="O12" s="45"/>
       <c r="P12" s="44" t="s">
@@ -2074,16 +2041,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S12" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T12" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="U12" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="T12" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -2103,19 +2070,19 @@
         <v>102</v>
       </c>
       <c r="F13" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G13" s="36" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="H13" s="37">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I13" s="37" t="s">
         <v>20</v>
       </c>
       <c r="J13" s="50" t="s">
-        <v>215</v>
+        <v>173</v>
       </c>
       <c r="K13" s="42" t="s">
         <v>69</v>
@@ -2125,7 +2092,7 @@
       </c>
       <c r="M13" s="46"/>
       <c r="N13" s="46" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="O13" s="45"/>
       <c r="P13" s="44" t="s">
@@ -2135,19 +2102,19 @@
         <v>6</v>
       </c>
       <c r="R13" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S13" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T13" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="U13" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="T13" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>67</v>
       </c>
@@ -2164,19 +2131,19 @@
         <v>102</v>
       </c>
       <c r="F14" s="30" t="s">
-        <v>174</v>
+        <v>104</v>
       </c>
       <c r="G14" s="36" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="H14" s="37">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I14" s="37" t="s">
         <v>20</v>
       </c>
       <c r="J14" s="50" t="s">
-        <v>178</v>
+        <v>213</v>
       </c>
       <c r="K14" s="42" t="s">
         <v>69</v>
@@ -2186,7 +2153,7 @@
       </c>
       <c r="M14" s="46"/>
       <c r="N14" s="46" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="O14" s="45"/>
       <c r="P14" s="44" t="s">
@@ -2196,22 +2163,19 @@
         <v>6</v>
       </c>
       <c r="R14" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S14" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T14" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="U14" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="T14" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="W14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:23" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>67</v>
       </c>
@@ -2228,19 +2192,19 @@
         <v>102</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="G15" s="36" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="H15" s="37">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I15" s="37" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="50" t="s">
-        <v>216</v>
+        <v>176</v>
       </c>
       <c r="K15" s="42" t="s">
         <v>69</v>
@@ -2250,7 +2214,7 @@
       </c>
       <c r="M15" s="46"/>
       <c r="N15" s="46" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="O15" s="45"/>
       <c r="P15" s="44" t="s">
@@ -2260,19 +2224,22 @@
         <v>6</v>
       </c>
       <c r="R15" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S15" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T15" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="U15" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="T15" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="U15" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>67</v>
       </c>
@@ -2292,16 +2259,16 @@
         <v>105</v>
       </c>
       <c r="G16" s="36" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="H16" s="37">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I16" s="37" t="s">
         <v>20</v>
       </c>
       <c r="J16" s="50" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="K16" s="42" t="s">
         <v>69</v>
@@ -2311,26 +2278,26 @@
       </c>
       <c r="M16" s="46"/>
       <c r="N16" s="46" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="O16" s="45"/>
       <c r="P16" s="44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q16" s="1">
         <v>6</v>
       </c>
       <c r="R16" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S16" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T16" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="U16" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="T16" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="U16" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2353,48 +2320,48 @@
         <v>105</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>130</v>
+        <v>197</v>
       </c>
       <c r="H17" s="37">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I17" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" s="38" t="s">
-        <v>132</v>
+        <v>20</v>
+      </c>
+      <c r="J17" s="50" t="s">
+        <v>199</v>
       </c>
       <c r="K17" s="42" t="s">
         <v>69</v>
       </c>
       <c r="L17" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="M17" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="N17" s="46"/>
+        <v>32</v>
+      </c>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46" t="s">
+        <v>23</v>
+      </c>
       <c r="O17" s="45"/>
       <c r="P17" s="44" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q17" s="1">
         <v>6</v>
       </c>
       <c r="R17" s="13" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="S17" s="13" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="T17" s="13" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>67</v>
       </c>
@@ -2408,49 +2375,51 @@
         <v>101</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="F18" s="30"/>
+        <v>102</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>105</v>
+      </c>
       <c r="G18" s="36" t="s">
-        <v>193</v>
+        <v>128</v>
       </c>
       <c r="H18" s="37">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I18" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J18" s="38" t="s">
-        <v>172</v>
+        <v>130</v>
       </c>
       <c r="K18" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L18" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M18" s="46"/>
+        <v>31</v>
+      </c>
+      <c r="M18" s="46" t="s">
+        <v>36</v>
+      </c>
       <c r="N18" s="46"/>
-      <c r="O18" s="45" t="s">
-        <v>173</v>
-      </c>
+      <c r="O18" s="45"/>
       <c r="P18" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="1" t="s">
-        <v>125</v>
+      <c r="Q18" s="1">
+        <v>6</v>
       </c>
       <c r="R18" s="13" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="S18" s="13" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="T18" s="13" t="s">
-        <v>171</v>
+        <v>133</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -2469,49 +2438,47 @@
       <c r="E19" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="F19" s="30" t="s">
-        <v>107</v>
-      </c>
+      <c r="F19" s="30"/>
       <c r="G19" s="36" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="H19" s="37">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I19" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="50" t="s">
-        <v>184</v>
+      <c r="J19" s="38" t="s">
+        <v>170</v>
       </c>
       <c r="K19" s="42" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L19" s="43" t="s">
         <v>32</v>
       </c>
       <c r="M19" s="46"/>
-      <c r="N19" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="O19" s="45"/>
+      <c r="N19" s="46"/>
+      <c r="O19" s="45" t="s">
+        <v>171</v>
+      </c>
       <c r="P19" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="1">
-        <v>6</v>
+      <c r="Q19" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="R19" s="13" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="S19" s="13" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="T19" s="13" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -2531,19 +2498,19 @@
         <v>106</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G20" s="36" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="H20" s="37">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I20" s="37" t="s">
         <v>20</v>
       </c>
       <c r="J20" s="50" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="K20" s="42" t="s">
         <v>69</v>
@@ -2553,7 +2520,7 @@
       </c>
       <c r="M20" s="46"/>
       <c r="N20" s="46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O20" s="45"/>
       <c r="P20" s="44" t="s">
@@ -2563,16 +2530,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S20" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T20" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="U20" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="T20" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="U20" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -2592,19 +2559,19 @@
         <v>106</v>
       </c>
       <c r="F21" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G21" s="36" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="H21" s="37">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I21" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="38" t="s">
-        <v>194</v>
+      <c r="J21" s="50" t="s">
+        <v>186</v>
       </c>
       <c r="K21" s="42" t="s">
         <v>69</v>
@@ -2614,7 +2581,7 @@
       </c>
       <c r="M21" s="46"/>
       <c r="N21" s="46" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="O21" s="45"/>
       <c r="P21" s="44" t="s">
@@ -2624,16 +2591,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S21" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T21" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="U21" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="T21" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="U21" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -2656,16 +2623,16 @@
         <v>109</v>
       </c>
       <c r="G22" s="36" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="H22" s="37">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I22" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="50" t="s">
-        <v>197</v>
+      <c r="J22" s="38" t="s">
+        <v>192</v>
       </c>
       <c r="K22" s="42" t="s">
         <v>69</v>
@@ -2675,7 +2642,7 @@
       </c>
       <c r="M22" s="46"/>
       <c r="N22" s="46" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="O22" s="45"/>
       <c r="P22" s="44" t="s">
@@ -2685,16 +2652,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S22" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T22" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="U22" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="T22" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -2717,16 +2684,16 @@
         <v>109</v>
       </c>
       <c r="G23" s="36" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="H23" s="37">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I23" s="37" t="s">
         <v>20</v>
       </c>
       <c r="J23" s="50" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="K23" s="42" t="s">
         <v>69</v>
@@ -2736,26 +2703,26 @@
       </c>
       <c r="M23" s="46"/>
       <c r="N23" s="46" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="O23" s="45"/>
       <c r="P23" s="44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q23" s="1">
         <v>6</v>
       </c>
       <c r="R23" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S23" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T23" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="U23" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="T23" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="U23" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -2778,45 +2745,45 @@
         <v>109</v>
       </c>
       <c r="G24" s="36" t="s">
-        <v>131</v>
+        <v>198</v>
       </c>
       <c r="H24" s="37">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I24" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="38" t="s">
-        <v>137</v>
+        <v>20</v>
+      </c>
+      <c r="J24" s="50" t="s">
+        <v>200</v>
       </c>
       <c r="K24" s="42" t="s">
         <v>69</v>
       </c>
       <c r="L24" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="M24" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="N24" s="46"/>
+        <v>32</v>
+      </c>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46" t="s">
+        <v>23</v>
+      </c>
       <c r="O24" s="45"/>
       <c r="P24" s="44" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q24" s="1">
         <v>6</v>
       </c>
       <c r="R24" s="13" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="S24" s="13" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="T24" s="13" t="s">
-        <v>138</v>
+        <v>201</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -2833,31 +2800,33 @@
         <v>101</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="F25" s="30"/>
+        <v>106</v>
+      </c>
+      <c r="F25" s="30" t="s">
+        <v>109</v>
+      </c>
       <c r="G25" s="36" t="s">
-        <v>204</v>
+        <v>129</v>
       </c>
       <c r="H25" s="37">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I25" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J25" s="38" t="s">
-        <v>205</v>
+        <v>135</v>
       </c>
       <c r="K25" s="42" t="s">
         <v>69</v>
       </c>
       <c r="L25" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46" t="s">
-        <v>23</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="M25" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="N25" s="46"/>
       <c r="O25" s="45"/>
       <c r="P25" s="44" t="s">
         <v>19</v>
@@ -2866,16 +2835,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="13" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="S25" s="13" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="T25" s="13" t="s">
-        <v>206</v>
+        <v>136</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -2892,20 +2861,20 @@
         <v>101</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="F26" s="30"/>
       <c r="G26" s="36" t="s">
-        <v>146</v>
+        <v>202</v>
       </c>
       <c r="H26" s="37">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I26" s="37" t="s">
         <v>20</v>
       </c>
       <c r="J26" s="38" t="s">
-        <v>147</v>
+        <v>203</v>
       </c>
       <c r="K26" s="42" t="s">
         <v>69</v>
@@ -2915,7 +2884,7 @@
       </c>
       <c r="M26" s="46"/>
       <c r="N26" s="46" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="O26" s="45"/>
       <c r="P26" s="44" t="s">
@@ -2925,16 +2894,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S26" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T26" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="U26" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="T26" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="U26" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -2948,27 +2917,53 @@
         <v>92</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F27" s="30"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="42"/>
-      <c r="L27" s="43"/>
+      <c r="G27" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="H27" s="37">
+        <v>21</v>
+      </c>
+      <c r="I27" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="J27" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="K27" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="L27" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="M27" s="46"/>
-      <c r="N27" s="46"/>
+      <c r="N27" s="46" t="s">
+        <v>62</v>
+      </c>
       <c r="O27" s="45"/>
-      <c r="P27" s="44"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="2"/>
+      <c r="P27" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>6</v>
+      </c>
+      <c r="R27" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="S27" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T27" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="U27" s="2" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
@@ -2984,7 +2979,7 @@
         <v>111</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F28" s="30"/>
       <c r="G28" s="36"/>
@@ -3017,7 +3012,7 @@
         <v>111</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F29" s="30"/>
       <c r="G29" s="36"/>
@@ -3050,50 +3045,24 @@
         <v>111</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F30" s="30"/>
-      <c r="G30" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="H30" s="37">
-        <v>22</v>
-      </c>
-      <c r="I30" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="J30" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="K30" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="L30" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="M30" s="46" t="s">
-        <v>44</v>
-      </c>
+      <c r="G30" s="36"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="46"/>
       <c r="N30" s="46"/>
       <c r="O30" s="45"/>
-      <c r="P30" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q30" s="1">
-        <v>6</v>
-      </c>
-      <c r="R30" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="S30" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="T30" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="U30" s="2" t="s">
-        <v>136</v>
-      </c>
+      <c r="P30" s="44"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="2"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
@@ -3109,31 +3078,31 @@
         <v>111</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="F31" s="30"/>
-      <c r="G31" s="50" t="s">
-        <v>149</v>
+      <c r="G31" s="36" t="s">
+        <v>115</v>
       </c>
       <c r="H31" s="37">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I31" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J31" s="38" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="K31" s="42" t="s">
         <v>69</v>
       </c>
       <c r="L31" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M31" s="46"/>
-      <c r="N31" s="46" t="s">
-        <v>62</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="M31" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="N31" s="46"/>
       <c r="O31" s="45"/>
       <c r="P31" s="44" t="s">
         <v>19</v>
@@ -3142,16 +3111,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="13" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="S31" s="13" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="T31" s="13" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="U31" s="2" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -3165,21 +3134,23 @@
         <v>92</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="E32" s="29"/>
+        <v>111</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>100</v>
+      </c>
       <c r="F32" s="30"/>
-      <c r="G32" s="36" t="s">
-        <v>152</v>
+      <c r="G32" s="50" t="s">
+        <v>147</v>
       </c>
       <c r="H32" s="37">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I32" s="37" t="s">
         <v>20</v>
       </c>
       <c r="J32" s="38" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="K32" s="42" t="s">
         <v>69</v>
@@ -3189,7 +3160,7 @@
       </c>
       <c r="M32" s="46"/>
       <c r="N32" s="46" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O32" s="45"/>
       <c r="P32" s="44" t="s">
@@ -3199,16 +3170,16 @@
         <v>6</v>
       </c>
       <c r="R32" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S32" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T32" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="U32" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="T32" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="U32" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -3227,16 +3198,16 @@
       <c r="E33" s="29"/>
       <c r="F33" s="30"/>
       <c r="G33" s="36" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H33" s="37">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I33" s="37" t="s">
         <v>20</v>
       </c>
       <c r="J33" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K33" s="42" t="s">
         <v>69</v>
@@ -3256,16 +3227,16 @@
         <v>6</v>
       </c>
       <c r="R33" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S33" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T33" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="U33" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="T33" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="U33" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -3284,16 +3255,16 @@
       <c r="E34" s="29"/>
       <c r="F34" s="30"/>
       <c r="G34" s="36" t="s">
-        <v>207</v>
+        <v>151</v>
       </c>
       <c r="H34" s="37">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I34" s="37" t="s">
         <v>20</v>
       </c>
       <c r="J34" s="38" t="s">
-        <v>208</v>
+        <v>152</v>
       </c>
       <c r="K34" s="42" t="s">
         <v>69</v>
@@ -3303,7 +3274,7 @@
       </c>
       <c r="M34" s="46"/>
       <c r="N34" s="46" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="O34" s="45"/>
       <c r="P34" s="44" t="s">
@@ -3313,16 +3284,16 @@
         <v>6</v>
       </c>
       <c r="R34" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S34" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T34" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="U34" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="T34" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="U34" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
@@ -3336,39 +3307,51 @@
         <v>92</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>158</v>
+        <v>116</v>
       </c>
       <c r="E35" s="29"/>
       <c r="F35" s="30"/>
       <c r="G35" s="36" t="s">
-        <v>159</v>
+        <v>205</v>
       </c>
       <c r="H35" s="37">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I35" s="37" t="s">
         <v>20</v>
       </c>
       <c r="J35" s="38" t="s">
-        <v>162</v>
+        <v>206</v>
       </c>
       <c r="K35" s="42" t="s">
         <v>69</v>
       </c>
       <c r="L35" s="43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M35" s="46"/>
-      <c r="N35" s="46"/>
+      <c r="N35" s="46" t="s">
+        <v>53</v>
+      </c>
       <c r="O35" s="45"/>
       <c r="P35" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q35" s="1"/>
-      <c r="R35" s="13"/>
-      <c r="S35" s="13"/>
-      <c r="T35" s="13"/>
-      <c r="U35" s="2"/>
+      <c r="Q35" s="1">
+        <v>6</v>
+      </c>
+      <c r="R35" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="S35" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T35" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="U35" s="2" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
@@ -3381,51 +3364,39 @@
         <v>92</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E36" s="29"/>
       <c r="F36" s="30"/>
       <c r="G36" s="36" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H36" s="37">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I36" s="37" t="s">
         <v>20</v>
       </c>
       <c r="J36" s="38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K36" s="42" t="s">
         <v>69</v>
       </c>
       <c r="L36" s="43" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M36" s="46"/>
-      <c r="N36" s="46" t="s">
-        <v>23</v>
-      </c>
+      <c r="N36" s="46"/>
       <c r="O36" s="45"/>
       <c r="P36" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q36" s="1">
-        <v>6</v>
-      </c>
-      <c r="R36" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="S36" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="T36" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="U36" s="2" t="s">
-        <v>145</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="2"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
@@ -3437,20 +3408,22 @@
       <c r="C37" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="D37" s="25"/>
+      <c r="D37" s="25" t="s">
+        <v>156</v>
+      </c>
       <c r="E37" s="29"/>
       <c r="F37" s="30"/>
       <c r="G37" s="36" t="s">
-        <v>212</v>
+        <v>158</v>
       </c>
       <c r="H37" s="37">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I37" s="37" t="s">
         <v>20</v>
       </c>
       <c r="J37" s="38" t="s">
-        <v>213</v>
+        <v>159</v>
       </c>
       <c r="K37" s="42" t="s">
         <v>69</v>
@@ -3460,50 +3433,82 @@
       </c>
       <c r="M37" s="46"/>
       <c r="N37" s="46" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="O37" s="45"/>
       <c r="P37" s="44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q37" s="1">
         <v>6</v>
       </c>
       <c r="R37" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S37" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T37" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="U37" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="T37" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="U37" s="2" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="24"/>
+      <c r="A38" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>92</v>
+      </c>
       <c r="D38" s="25"/>
       <c r="E38" s="29"/>
       <c r="F38" s="30"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="42"/>
-      <c r="L38" s="43"/>
+      <c r="G38" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="H38" s="37">
+        <v>29</v>
+      </c>
+      <c r="I38" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="K38" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="L38" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="M38" s="46"/>
-      <c r="N38" s="46"/>
+      <c r="N38" s="46" t="s">
+        <v>63</v>
+      </c>
       <c r="O38" s="45"/>
-      <c r="P38" s="44"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="13"/>
-      <c r="S38" s="13"/>
-      <c r="T38" s="13"/>
-      <c r="U38" s="2"/>
+      <c r="P38" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>6</v>
+      </c>
+      <c r="R38" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="S38" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="T38" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="U38" s="2" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
@@ -3512,7 +3517,7 @@
       <c r="D39" s="25"/>
       <c r="E39" s="29"/>
       <c r="F39" s="30"/>
-      <c r="G39" s="36"/>
+      <c r="G39" s="39"/>
       <c r="H39" s="37"/>
       <c r="I39" s="37"/>
       <c r="J39" s="38"/>
@@ -3630,7 +3635,7 @@
       <c r="G44" s="36"/>
       <c r="H44" s="37"/>
       <c r="I44" s="37"/>
-      <c r="J44" s="35"/>
+      <c r="J44" s="38"/>
       <c r="K44" s="42"/>
       <c r="L44" s="43"/>
       <c r="M44" s="46"/>
@@ -3653,7 +3658,7 @@
       <c r="G45" s="36"/>
       <c r="H45" s="37"/>
       <c r="I45" s="37"/>
-      <c r="J45" s="38"/>
+      <c r="J45" s="35"/>
       <c r="K45" s="42"/>
       <c r="L45" s="43"/>
       <c r="M45" s="46"/>
@@ -3758,7 +3763,7 @@
       <c r="T49" s="13"/>
       <c r="U49" s="2"/>
     </row>
-    <row r="50" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="22"/>
       <c r="B50" s="23"/>
       <c r="C50" s="24"/>
@@ -3781,7 +3786,7 @@
       <c r="T50" s="13"/>
       <c r="U50" s="2"/>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="22"/>
       <c r="B51" s="23"/>
       <c r="C51" s="24"/>
@@ -3854,9 +3859,9 @@
       <c r="A54" s="22"/>
       <c r="B54" s="23"/>
       <c r="C54" s="24"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="32"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="30"/>
       <c r="G54" s="36"/>
       <c r="H54" s="37"/>
       <c r="I54" s="37"/>
@@ -4908,8 +4913,36 @@
       <c r="T99" s="13"/>
       <c r="U99" s="2"/>
     </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A100" s="22"/>
+      <c r="B100" s="23"/>
+      <c r="C100" s="24"/>
+      <c r="D100" s="26"/>
+      <c r="E100" s="31"/>
+      <c r="F100" s="32"/>
+      <c r="G100" s="36"/>
+      <c r="H100" s="37"/>
+      <c r="I100" s="37"/>
+      <c r="J100" s="38"/>
+      <c r="K100" s="42"/>
+      <c r="L100" s="43"/>
+      <c r="M100" s="46"/>
+      <c r="N100" s="46"/>
+      <c r="O100" s="45"/>
+      <c r="P100" s="44"/>
+      <c r="Q100" s="1"/>
+      <c r="R100" s="13"/>
+      <c r="S100" s="13"/>
+      <c r="T100" s="13"/>
+      <c r="U100" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="U1:U2"/>
@@ -4925,11 +4958,6 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4940,37 +4968,37 @@
           <x14:formula1>
             <xm:f>DATOS!$D$2:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A99</xm:sqref>
+          <xm:sqref>A3:A100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K99</xm:sqref>
+          <xm:sqref>K3:K100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$F$2:$F$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L99</xm:sqref>
+          <xm:sqref>L3:L100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P3:P99</xm:sqref>
+          <xm:sqref>P3:P100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$C$2:$C$39</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N99</xm:sqref>
+          <xm:sqref>N3:N100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$2:$B$14</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M99</xm:sqref>
+          <xm:sqref>M3:M100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Modificaciones descripción de recursos
Modificaciones descripción de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion09/ESCALETAFINAL CN_09_09_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion09/ESCALETAFINAL CN_09_09_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado09\guion09\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -439,9 +444,6 @@
     <t>Recurso F6-02</t>
   </si>
   <si>
-    <t>Interactivo con animación incluida que permite explicar la ósmosis y la presión osmótica</t>
-  </si>
-  <si>
     <t>Recurso F12-01</t>
   </si>
   <si>
@@ -481,12 +483,6 @@
     <t xml:space="preserve">Competencias: preparación de disoluciones y diluciones </t>
   </si>
   <si>
-    <t>Competencias: preparación de un perfume</t>
-  </si>
-  <si>
-    <t>Actividad que propone una práctica de laboratorio para preparar un perfume</t>
-  </si>
-  <si>
     <t>Actividad que propone una práctica de laboratorio para preparar disoluciones y diluciones</t>
   </si>
   <si>
@@ -674,6 +670,15 @@
   </si>
   <si>
     <t>Secuencia de imágenes que permite explicar las caracteristicas de las disoluciones y el proceso de disolución</t>
+  </si>
+  <si>
+    <t>Animación que permite explicar la ósmosis y la presión osmótica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Competencias: preparación de un producto de cuidado personal </t>
+  </si>
+  <si>
+    <t>Actividad que propone una práctica de laboratorio para preparar agua de colonia</t>
   </si>
 </sst>
 </file>
@@ -1434,7 +1439,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1444,8 +1449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="G16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,7 +1625,7 @@
         <v>19</v>
       </c>
       <c r="J4" s="38" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="K4" s="42" t="s">
         <v>69</v>
@@ -1830,7 +1835,7 @@
       </c>
       <c r="F9" s="30"/>
       <c r="G9" s="36" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H9" s="37">
         <v>3</v>
@@ -1839,7 +1844,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="38" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K9" s="42" t="s">
         <v>69</v>
@@ -1862,13 +1867,13 @@
         <v>118</v>
       </c>
       <c r="S9" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T9" s="13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -1889,7 +1894,7 @@
       </c>
       <c r="F10" s="30"/>
       <c r="G10" s="36" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H10" s="37">
         <v>4</v>
@@ -1898,7 +1903,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="38" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K10" s="42" t="s">
         <v>70</v>
@@ -1922,7 +1927,7 @@
         <v>125</v>
       </c>
       <c r="T10" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="U10" s="2" t="s">
         <v>127</v>
@@ -1946,7 +1951,7 @@
       </c>
       <c r="F11" s="30"/>
       <c r="G11" s="51" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H11" s="37">
         <v>5</v>
@@ -1955,7 +1960,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="38" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="K11" s="42" t="s">
         <v>69</v>
@@ -1978,13 +1983,13 @@
         <v>118</v>
       </c>
       <c r="S11" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T11" s="13" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -2005,7 +2010,7 @@
       </c>
       <c r="F12" s="28"/>
       <c r="G12" s="36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H12" s="37">
         <v>6</v>
@@ -2014,7 +2019,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K12" s="42" t="s">
         <v>69</v>
@@ -2037,13 +2042,13 @@
         <v>118</v>
       </c>
       <c r="S12" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="T12" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="T12" s="13" t="s">
+      <c r="U12" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -2066,7 +2071,7 @@
         <v>103</v>
       </c>
       <c r="G13" s="36" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H13" s="37">
         <v>7</v>
@@ -2075,7 +2080,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="50" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K13" s="42" t="s">
         <v>69</v>
@@ -2098,13 +2103,13 @@
         <v>118</v>
       </c>
       <c r="S13" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T13" s="13" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -2127,7 +2132,7 @@
         <v>104</v>
       </c>
       <c r="G14" s="36" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H14" s="37">
         <v>8</v>
@@ -2136,7 +2141,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="50" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K14" s="42" t="s">
         <v>69</v>
@@ -2159,13 +2164,13 @@
         <v>118</v>
       </c>
       <c r="S14" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T14" s="13" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2185,10 +2190,10 @@
         <v>102</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G15" s="36" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H15" s="37">
         <v>9</v>
@@ -2197,7 +2202,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="50" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K15" s="42" t="s">
         <v>69</v>
@@ -2220,13 +2225,13 @@
         <v>118</v>
       </c>
       <c r="S15" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T15" s="13" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="W15" t="s">
         <v>90</v>
@@ -2252,7 +2257,7 @@
         <v>105</v>
       </c>
       <c r="G16" s="36" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H16" s="37">
         <v>10</v>
@@ -2261,7 +2266,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="50" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K16" s="42" t="s">
         <v>69</v>
@@ -2284,13 +2289,13 @@
         <v>118</v>
       </c>
       <c r="S16" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T16" s="13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2313,7 +2318,7 @@
         <v>105</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H17" s="37">
         <v>11</v>
@@ -2322,7 +2327,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="50" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="K17" s="42" t="s">
         <v>69</v>
@@ -2345,13 +2350,13 @@
         <v>118</v>
       </c>
       <c r="S17" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T17" s="13" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2415,7 +2420,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>67</v>
       </c>
@@ -2433,7 +2438,7 @@
       </c>
       <c r="F19" s="30"/>
       <c r="G19" s="36" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H19" s="37">
         <v>13</v>
@@ -2442,7 +2447,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="38" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K19" s="42" t="s">
         <v>70</v>
@@ -2453,7 +2458,7 @@
       <c r="M19" s="46"/>
       <c r="N19" s="46"/>
       <c r="O19" s="45" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="P19" s="44" t="s">
         <v>19</v>
@@ -2468,7 +2473,7 @@
         <v>125</v>
       </c>
       <c r="T19" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="U19" s="2" t="s">
         <v>127</v>
@@ -2494,7 +2499,7 @@
         <v>107</v>
       </c>
       <c r="G20" s="36" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H20" s="37">
         <v>14</v>
@@ -2503,7 +2508,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="50" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K20" s="42" t="s">
         <v>69</v>
@@ -2526,13 +2531,13 @@
         <v>118</v>
       </c>
       <c r="S20" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T20" s="13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -2555,7 +2560,7 @@
         <v>108</v>
       </c>
       <c r="G21" s="36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H21" s="37">
         <v>15</v>
@@ -2564,7 +2569,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="50" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="K21" s="42" t="s">
         <v>69</v>
@@ -2587,13 +2592,13 @@
         <v>118</v>
       </c>
       <c r="S21" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T21" s="13" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -2616,7 +2621,7 @@
         <v>109</v>
       </c>
       <c r="G22" s="36" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H22" s="37">
         <v>16</v>
@@ -2625,7 +2630,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="38" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="K22" s="42" t="s">
         <v>69</v>
@@ -2648,13 +2653,13 @@
         <v>118</v>
       </c>
       <c r="S22" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T22" s="13" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -2677,7 +2682,7 @@
         <v>109</v>
       </c>
       <c r="G23" s="36" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H23" s="37">
         <v>17</v>
@@ -2686,7 +2691,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="50" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="K23" s="42" t="s">
         <v>69</v>
@@ -2709,13 +2714,13 @@
         <v>118</v>
       </c>
       <c r="S23" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T23" s="13" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -2738,7 +2743,7 @@
         <v>109</v>
       </c>
       <c r="G24" s="36" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H24" s="37">
         <v>18</v>
@@ -2747,7 +2752,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="50" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K24" s="42" t="s">
         <v>69</v>
@@ -2770,13 +2775,13 @@
         <v>118</v>
       </c>
       <c r="S24" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T24" s="13" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -2858,7 +2863,7 @@
       </c>
       <c r="F26" s="30"/>
       <c r="G26" s="36" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H26" s="37">
         <v>20</v>
@@ -2867,7 +2872,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="38" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="K26" s="42" t="s">
         <v>69</v>
@@ -2890,13 +2895,13 @@
         <v>118</v>
       </c>
       <c r="S26" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T26" s="13" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="U26" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -2917,7 +2922,7 @@
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H27" s="37">
         <v>21</v>
@@ -2926,7 +2931,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K27" s="42" t="s">
         <v>69</v>
@@ -2949,13 +2954,13 @@
         <v>118</v>
       </c>
       <c r="S27" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T27" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="U27" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
@@ -3084,7 +3089,7 @@
         <v>19</v>
       </c>
       <c r="J31" s="38" t="s">
-        <v>137</v>
+        <v>213</v>
       </c>
       <c r="K31" s="42" t="s">
         <v>69</v>
@@ -3110,7 +3115,7 @@
         <v>132</v>
       </c>
       <c r="T31" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U31" s="2" t="s">
         <v>134</v>
@@ -3134,7 +3139,7 @@
       </c>
       <c r="F32" s="30"/>
       <c r="G32" s="50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H32" s="37">
         <v>23</v>
@@ -3143,7 +3148,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K32" s="42" t="s">
         <v>69</v>
@@ -3166,13 +3171,13 @@
         <v>118</v>
       </c>
       <c r="S32" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T32" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -3191,7 +3196,7 @@
       <c r="E33" s="29"/>
       <c r="F33" s="30"/>
       <c r="G33" s="36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H33" s="37">
         <v>24</v>
@@ -3200,7 +3205,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="38" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K33" s="42" t="s">
         <v>69</v>
@@ -3223,13 +3228,13 @@
         <v>118</v>
       </c>
       <c r="S33" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T33" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="U33" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -3248,7 +3253,7 @@
       <c r="E34" s="29"/>
       <c r="F34" s="30"/>
       <c r="G34" s="36" t="s">
-        <v>151</v>
+        <v>214</v>
       </c>
       <c r="H34" s="37">
         <v>25</v>
@@ -3257,7 +3262,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="38" t="s">
-        <v>152</v>
+        <v>215</v>
       </c>
       <c r="K34" s="42" t="s">
         <v>69</v>
@@ -3280,13 +3285,13 @@
         <v>118</v>
       </c>
       <c r="S34" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T34" s="13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="U34" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
@@ -3305,7 +3310,7 @@
       <c r="E35" s="29"/>
       <c r="F35" s="30"/>
       <c r="G35" s="36" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H35" s="37">
         <v>26</v>
@@ -3314,7 +3319,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="38" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="K35" s="42" t="s">
         <v>69</v>
@@ -3337,13 +3342,13 @@
         <v>118</v>
       </c>
       <c r="S35" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T35" s="13" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="U35" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
@@ -3357,12 +3362,12 @@
         <v>92</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E36" s="29"/>
       <c r="F36" s="30"/>
       <c r="G36" s="36" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H36" s="37">
         <v>27</v>
@@ -3371,7 +3376,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="38" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K36" s="42" t="s">
         <v>69</v>
@@ -3402,12 +3407,12 @@
         <v>92</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E37" s="29"/>
       <c r="F37" s="30"/>
       <c r="G37" s="36" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H37" s="37">
         <v>28</v>
@@ -3416,7 +3421,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="38" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K37" s="42" t="s">
         <v>69</v>
@@ -3439,13 +3444,13 @@
         <v>118</v>
       </c>
       <c r="S37" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T37" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="U37" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -3462,7 +3467,7 @@
       <c r="E38" s="29"/>
       <c r="F38" s="30"/>
       <c r="G38" s="36" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H38" s="37">
         <v>29</v>
@@ -3471,7 +3476,7 @@
         <v>20</v>
       </c>
       <c r="J38" s="38" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="K38" s="42" t="s">
         <v>69</v>
@@ -3494,13 +3499,13 @@
         <v>118</v>
       </c>
       <c r="S38" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T38" s="13" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="U38" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
@@ -4931,11 +4936,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="U1:U2"/>
@@ -4951,6 +4951,11 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambio de lugar en recursos
Cambio de lugar en recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion09/ESCALETAFINAL CN_09_09_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion09/ESCALETAFINAL CN_09_09_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado09\guion09\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="216">
   <si>
     <t>Asignatura</t>
   </si>
@@ -721,7 +721,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -767,6 +767,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1059,7 +1071,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1136,12 +1148,61 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1166,6 +1227,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1447,10 +1511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W100"/>
+  <dimension ref="A1:AZ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,97 +1541,102 @@
     <col min="21" max="21" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="K1" s="88" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="L1" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="59" t="s">
+      <c r="M1" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="60"/>
-      <c r="O1" s="53" t="s">
+      <c r="N1" s="91"/>
+      <c r="O1" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="53" t="s">
+      <c r="P1" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="53" t="s">
+      <c r="Q1" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="53" t="s">
+      <c r="R1" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="53" t="s">
+      <c r="S1" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="53" t="s">
+      <c r="T1" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="53" t="s">
+      <c r="U1" s="84" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="12" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="52" t="s">
+    <row r="2" spans="1:52" s="12" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="85"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="51" t="s">
         <v>87</v>
       </c>
       <c r="N2" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-    </row>
-    <row r="3" spans="1:23" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="85"/>
+      <c r="U2" s="85"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+    </row>
+    <row r="3" spans="1:52" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>67</v>
       </c>
@@ -1598,7 +1667,7 @@
       <c r="T3" s="14"/>
       <c r="U3" s="4"/>
     </row>
-    <row r="4" spans="1:23" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>67</v>
       </c>
@@ -1657,7 +1726,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>67</v>
       </c>
@@ -1692,7 +1761,7 @@
       <c r="T5" s="13"/>
       <c r="U5" s="2"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>67</v>
       </c>
@@ -1711,7 +1780,7 @@
       <c r="F6" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G6" s="51"/>
+      <c r="G6" s="50"/>
       <c r="H6" s="37"/>
       <c r="I6" s="37"/>
       <c r="J6" s="38"/>
@@ -1727,7 +1796,7 @@
       <c r="T6" s="13"/>
       <c r="U6" s="2"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>67</v>
       </c>
@@ -1760,7 +1829,7 @@
       <c r="T7" s="13"/>
       <c r="U7" s="2"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>67</v>
       </c>
@@ -1817,7 +1886,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>67</v>
       </c>
@@ -1876,7 +1945,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>67</v>
       </c>
@@ -1933,7 +2002,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>67</v>
       </c>
@@ -1950,7 +2019,7 @@
         <v>99</v>
       </c>
       <c r="F11" s="30"/>
-      <c r="G11" s="51" t="s">
+      <c r="G11" s="50" t="s">
         <v>158</v>
       </c>
       <c r="H11" s="37">
@@ -1992,7 +2061,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>67</v>
       </c>
@@ -2051,808 +2120,1206 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="1:52" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="F13" s="30" t="s">
+      <c r="F13" s="57"/>
+      <c r="G13" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" s="58">
+        <v>7</v>
+      </c>
+      <c r="I13" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="59" t="s">
+        <v>130</v>
+      </c>
+      <c r="K13" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="M13" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="N13" s="61"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13" s="64">
+        <v>6</v>
+      </c>
+      <c r="R13" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="S13" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="T13" s="65" t="s">
+        <v>133</v>
+      </c>
+      <c r="U13" s="66" t="s">
+        <v>134</v>
+      </c>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="Y13"/>
+      <c r="Z13"/>
+      <c r="AA13"/>
+      <c r="AB13"/>
+      <c r="AC13"/>
+      <c r="AD13"/>
+      <c r="AE13"/>
+      <c r="AF13"/>
+      <c r="AG13"/>
+      <c r="AH13"/>
+      <c r="AI13"/>
+      <c r="AJ13"/>
+      <c r="AK13"/>
+      <c r="AL13"/>
+      <c r="AM13"/>
+      <c r="AN13"/>
+      <c r="AO13"/>
+      <c r="AP13"/>
+      <c r="AQ13"/>
+      <c r="AR13"/>
+      <c r="AS13"/>
+      <c r="AT13"/>
+      <c r="AU13"/>
+      <c r="AV13"/>
+      <c r="AW13"/>
+      <c r="AX13"/>
+      <c r="AY13"/>
+      <c r="AZ13"/>
+    </row>
+    <row r="14" spans="1:52" s="82" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="70" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="71" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="73" t="s">
         <v>103</v>
       </c>
-      <c r="G13" s="36" t="s">
+      <c r="G14" s="71" t="s">
         <v>185</v>
       </c>
-      <c r="H13" s="37">
-        <v>7</v>
-      </c>
-      <c r="I13" s="37" t="s">
+      <c r="H14" s="74">
+        <v>8</v>
+      </c>
+      <c r="I14" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="50" t="s">
+      <c r="J14" s="83" t="s">
         <v>170</v>
       </c>
-      <c r="K13" s="42" t="s">
+      <c r="K14" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="L13" s="43" t="s">
+      <c r="L14" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M13" s="46"/>
-      <c r="N13" s="46" t="s">
+      <c r="M14" s="76"/>
+      <c r="N14" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="O13" s="45"/>
-      <c r="P13" s="44" t="s">
+      <c r="O14" s="77"/>
+      <c r="P14" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="Q14" s="79">
         <v>6</v>
       </c>
-      <c r="R13" s="13" t="s">
+      <c r="R14" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="S13" s="13" t="s">
+      <c r="S14" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="T13" s="13" t="s">
+      <c r="T14" s="80" t="s">
         <v>171</v>
       </c>
-      <c r="U13" s="2" t="s">
+      <c r="U14" s="81" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+      <c r="AB14"/>
+      <c r="AC14"/>
+      <c r="AD14"/>
+      <c r="AE14"/>
+      <c r="AF14"/>
+      <c r="AG14"/>
+      <c r="AH14"/>
+      <c r="AI14"/>
+      <c r="AJ14"/>
+      <c r="AK14"/>
+      <c r="AL14"/>
+      <c r="AM14"/>
+      <c r="AN14"/>
+      <c r="AO14"/>
+      <c r="AP14"/>
+      <c r="AQ14"/>
+      <c r="AR14"/>
+      <c r="AS14"/>
+      <c r="AT14"/>
+      <c r="AU14"/>
+      <c r="AV14"/>
+      <c r="AW14"/>
+      <c r="AX14"/>
+      <c r="AY14"/>
+      <c r="AZ14"/>
+    </row>
+    <row r="15" spans="1:52" s="82" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B15" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C15" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D15" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E15" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F15" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G15" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="H14" s="37">
-        <v>8</v>
-      </c>
-      <c r="I14" s="37" t="s">
+      <c r="H15" s="74">
+        <v>9</v>
+      </c>
+      <c r="I15" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="50" t="s">
+      <c r="J15" s="83" t="s">
         <v>208</v>
       </c>
-      <c r="K14" s="42" t="s">
+      <c r="K15" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="L14" s="43" t="s">
+      <c r="L15" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M14" s="46"/>
-      <c r="N14" s="46" t="s">
+      <c r="M15" s="76"/>
+      <c r="N15" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="O14" s="45"/>
-      <c r="P14" s="44" t="s">
+      <c r="O15" s="77"/>
+      <c r="P15" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="Q15" s="79">
         <v>6</v>
       </c>
-      <c r="R14" s="13" t="s">
+      <c r="R15" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="S14" s="13" t="s">
+      <c r="S15" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="T14" s="13" t="s">
+      <c r="T15" s="80" t="s">
         <v>179</v>
       </c>
-      <c r="U14" s="2" t="s">
+      <c r="U15" s="81" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
+      <c r="Z15"/>
+      <c r="AA15"/>
+      <c r="AB15"/>
+      <c r="AC15"/>
+      <c r="AD15"/>
+      <c r="AE15"/>
+      <c r="AF15"/>
+      <c r="AG15"/>
+      <c r="AH15"/>
+      <c r="AI15"/>
+      <c r="AJ15"/>
+      <c r="AK15"/>
+      <c r="AL15"/>
+      <c r="AM15"/>
+      <c r="AN15"/>
+      <c r="AO15"/>
+      <c r="AP15"/>
+      <c r="AQ15"/>
+      <c r="AR15"/>
+      <c r="AS15"/>
+      <c r="AT15"/>
+      <c r="AU15"/>
+      <c r="AV15"/>
+      <c r="AW15"/>
+      <c r="AX15"/>
+      <c r="AY15"/>
+      <c r="AZ15"/>
+    </row>
+    <row r="16" spans="1:52" s="82" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B16" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C16" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D16" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E16" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F16" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G16" s="71" t="s">
         <v>214</v>
       </c>
-      <c r="H15" s="37">
-        <v>9</v>
-      </c>
-      <c r="I15" s="37" t="s">
+      <c r="H16" s="74">
+        <v>10</v>
+      </c>
+      <c r="I16" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="50" t="s">
+      <c r="J16" s="83" t="s">
         <v>215</v>
       </c>
-      <c r="K15" s="42" t="s">
+      <c r="K16" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="L15" s="43" t="s">
+      <c r="L16" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M15" s="46"/>
-      <c r="N15" s="46" t="s">
+      <c r="M16" s="76"/>
+      <c r="N16" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="45"/>
-      <c r="P15" s="44" t="s">
+      <c r="O16" s="77"/>
+      <c r="P16" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="Q16" s="79">
         <v>6</v>
       </c>
-      <c r="R15" s="13" t="s">
+      <c r="R16" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="S15" s="13" t="s">
+      <c r="S16" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="T15" s="13" t="s">
+      <c r="T16" s="80" t="s">
         <v>173</v>
       </c>
-      <c r="U15" s="2" t="s">
+      <c r="U16" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="W15" t="s">
+      <c r="V16"/>
+      <c r="W16" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="X16"/>
+      <c r="Y16"/>
+      <c r="Z16"/>
+      <c r="AA16"/>
+      <c r="AB16"/>
+      <c r="AC16"/>
+      <c r="AD16"/>
+      <c r="AE16"/>
+      <c r="AF16"/>
+      <c r="AG16"/>
+      <c r="AH16"/>
+      <c r="AI16"/>
+      <c r="AJ16"/>
+      <c r="AK16"/>
+      <c r="AL16"/>
+      <c r="AM16"/>
+      <c r="AN16"/>
+      <c r="AO16"/>
+      <c r="AP16"/>
+      <c r="AQ16"/>
+      <c r="AR16"/>
+      <c r="AS16"/>
+      <c r="AT16"/>
+      <c r="AU16"/>
+      <c r="AV16"/>
+      <c r="AW16"/>
+      <c r="AX16"/>
+      <c r="AY16"/>
+      <c r="AZ16"/>
+    </row>
+    <row r="17" spans="1:52" s="82" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B17" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C17" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D17" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E17" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F17" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="G16" s="36" t="s">
+      <c r="G17" s="71" t="s">
         <v>174</v>
       </c>
-      <c r="H16" s="37">
-        <v>10</v>
-      </c>
-      <c r="I16" s="37" t="s">
+      <c r="H17" s="74">
+        <v>11</v>
+      </c>
+      <c r="I17" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="50" t="s">
+      <c r="J17" s="83" t="s">
         <v>209</v>
       </c>
-      <c r="K16" s="42" t="s">
+      <c r="K17" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="L16" s="43" t="s">
+      <c r="L17" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M16" s="46"/>
-      <c r="N16" s="46" t="s">
+      <c r="M17" s="76"/>
+      <c r="N17" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="O16" s="45"/>
-      <c r="P16" s="44" t="s">
+      <c r="O17" s="77"/>
+      <c r="P17" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="Q17" s="79">
         <v>6</v>
       </c>
-      <c r="R16" s="13" t="s">
+      <c r="R17" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="S16" s="13" t="s">
+      <c r="S17" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="T16" s="13" t="s">
+      <c r="T17" s="80" t="s">
         <v>175</v>
       </c>
-      <c r="U16" s="2" t="s">
+      <c r="U17" s="81" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
+      <c r="AA17"/>
+      <c r="AB17"/>
+      <c r="AC17"/>
+      <c r="AD17"/>
+      <c r="AE17"/>
+      <c r="AF17"/>
+      <c r="AG17"/>
+      <c r="AH17"/>
+      <c r="AI17"/>
+      <c r="AJ17"/>
+      <c r="AK17"/>
+      <c r="AL17"/>
+      <c r="AM17"/>
+      <c r="AN17"/>
+      <c r="AO17"/>
+      <c r="AP17"/>
+      <c r="AQ17"/>
+      <c r="AR17"/>
+      <c r="AS17"/>
+      <c r="AT17"/>
+      <c r="AU17"/>
+      <c r="AV17"/>
+      <c r="AW17"/>
+      <c r="AX17"/>
+      <c r="AY17"/>
+      <c r="AZ17"/>
+    </row>
+    <row r="18" spans="1:52" s="82" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B18" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C18" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D18" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E18" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F18" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="G17" s="36" t="s">
+      <c r="G18" s="71" t="s">
         <v>192</v>
       </c>
-      <c r="H17" s="37">
-        <v>11</v>
-      </c>
-      <c r="I17" s="37" t="s">
+      <c r="H18" s="74">
+        <v>12</v>
+      </c>
+      <c r="I18" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="50" t="s">
+      <c r="J18" s="83" t="s">
         <v>194</v>
       </c>
-      <c r="K17" s="42" t="s">
+      <c r="K18" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="L17" s="43" t="s">
+      <c r="L18" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46" t="s">
+      <c r="M18" s="76"/>
+      <c r="N18" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="O17" s="45"/>
-      <c r="P17" s="44" t="s">
+      <c r="O18" s="77"/>
+      <c r="P18" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="Q18" s="79">
         <v>6</v>
       </c>
-      <c r="R17" s="13" t="s">
+      <c r="R18" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="S17" s="13" t="s">
+      <c r="S18" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="T17" s="13" t="s">
+      <c r="T18" s="80" t="s">
         <v>176</v>
       </c>
-      <c r="U17" s="2" t="s">
+      <c r="U18" s="81" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+      <c r="Z18"/>
+      <c r="AA18"/>
+      <c r="AB18"/>
+      <c r="AC18"/>
+      <c r="AD18"/>
+      <c r="AE18"/>
+      <c r="AF18"/>
+      <c r="AG18"/>
+      <c r="AH18"/>
+      <c r="AI18"/>
+      <c r="AJ18"/>
+      <c r="AK18"/>
+      <c r="AL18"/>
+      <c r="AM18"/>
+      <c r="AN18"/>
+      <c r="AO18"/>
+      <c r="AP18"/>
+      <c r="AQ18"/>
+      <c r="AR18"/>
+      <c r="AS18"/>
+      <c r="AT18"/>
+      <c r="AU18"/>
+      <c r="AV18"/>
+      <c r="AW18"/>
+      <c r="AX18"/>
+      <c r="AY18"/>
+      <c r="AZ18"/>
+    </row>
+    <row r="19" spans="1:52" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B19" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C19" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D19" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="E18" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="F18" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="G18" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="H18" s="37">
-        <v>12</v>
-      </c>
-      <c r="I18" s="37" t="s">
+      <c r="E19" s="56" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="57"/>
+      <c r="G19" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="58">
+        <v>13</v>
+      </c>
+      <c r="I19" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="K18" s="42" t="s">
+      <c r="J19" s="59" t="s">
+        <v>135</v>
+      </c>
+      <c r="K19" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="L18" s="43" t="s">
+      <c r="L19" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="M18" s="46" t="s">
+      <c r="M19" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="N18" s="46"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="44" t="s">
+      <c r="N19" s="61"/>
+      <c r="O19" s="62"/>
+      <c r="P19" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="Q19" s="64">
         <v>6</v>
       </c>
-      <c r="R18" s="13" t="s">
+      <c r="R19" s="65" t="s">
         <v>131</v>
       </c>
-      <c r="S18" s="13" t="s">
+      <c r="S19" s="65" t="s">
         <v>132</v>
       </c>
-      <c r="T18" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="U18" s="2" t="s">
+      <c r="T19" s="65" t="s">
+        <v>136</v>
+      </c>
+      <c r="U19" s="66" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+      <c r="AB19"/>
+      <c r="AC19"/>
+      <c r="AD19"/>
+      <c r="AE19"/>
+      <c r="AF19"/>
+      <c r="AG19"/>
+      <c r="AH19"/>
+      <c r="AI19"/>
+      <c r="AJ19"/>
+      <c r="AK19"/>
+      <c r="AL19"/>
+      <c r="AM19"/>
+      <c r="AN19"/>
+      <c r="AO19"/>
+      <c r="AP19"/>
+      <c r="AQ19"/>
+      <c r="AR19"/>
+      <c r="AS19"/>
+      <c r="AT19"/>
+      <c r="AU19"/>
+      <c r="AV19"/>
+      <c r="AW19"/>
+      <c r="AX19"/>
+      <c r="AY19"/>
+      <c r="AZ19"/>
+    </row>
+    <row r="20" spans="1:52" s="82" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B20" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C20" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D20" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="29" t="s">
+      <c r="E20" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="F19" s="30"/>
-      <c r="G19" s="36" t="s">
+      <c r="F20" s="73"/>
+      <c r="G20" s="71" t="s">
         <v>186</v>
       </c>
-      <c r="H19" s="37">
-        <v>13</v>
-      </c>
-      <c r="I19" s="37" t="s">
+      <c r="H20" s="74">
+        <v>14</v>
+      </c>
+      <c r="I20" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="38" t="s">
+      <c r="J20" s="92" t="s">
         <v>167</v>
       </c>
-      <c r="K19" s="42" t="s">
+      <c r="K20" s="72" t="s">
         <v>70</v>
       </c>
-      <c r="L19" s="43" t="s">
+      <c r="L20" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="45" t="s">
+      <c r="M20" s="76"/>
+      <c r="N20" s="76"/>
+      <c r="O20" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="P19" s="44" t="s">
+      <c r="P20" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="Q20" s="79" t="s">
         <v>123</v>
       </c>
-      <c r="R19" s="13" t="s">
+      <c r="R20" s="80" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="13" t="s">
+      <c r="S20" s="80" t="s">
         <v>125</v>
       </c>
-      <c r="T19" s="13" t="s">
+      <c r="T20" s="80" t="s">
         <v>166</v>
       </c>
-      <c r="U19" s="2" t="s">
+      <c r="U20" s="81" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
+      <c r="Z20"/>
+      <c r="AA20"/>
+      <c r="AB20"/>
+      <c r="AC20"/>
+      <c r="AD20"/>
+      <c r="AE20"/>
+      <c r="AF20"/>
+      <c r="AG20"/>
+      <c r="AH20"/>
+      <c r="AI20"/>
+      <c r="AJ20"/>
+      <c r="AK20"/>
+      <c r="AL20"/>
+      <c r="AM20"/>
+      <c r="AN20"/>
+      <c r="AO20"/>
+      <c r="AP20"/>
+      <c r="AQ20"/>
+      <c r="AR20"/>
+      <c r="AS20"/>
+      <c r="AT20"/>
+      <c r="AU20"/>
+      <c r="AV20"/>
+      <c r="AW20"/>
+      <c r="AX20"/>
+      <c r="AY20"/>
+      <c r="AZ20"/>
+    </row>
+    <row r="21" spans="1:52" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B21" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C21" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D21" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="E20" s="29" t="s">
+      <c r="E21" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="F21" s="73" t="s">
         <v>107</v>
       </c>
-      <c r="G20" s="36" t="s">
+      <c r="G21" s="71" t="s">
         <v>177</v>
       </c>
-      <c r="H20" s="37">
-        <v>14</v>
-      </c>
-      <c r="I20" s="37" t="s">
+      <c r="H21" s="74">
+        <v>15</v>
+      </c>
+      <c r="I21" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="50" t="s">
+      <c r="J21" s="83" t="s">
         <v>178</v>
       </c>
-      <c r="K20" s="42" t="s">
+      <c r="K21" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="L20" s="43" t="s">
+      <c r="L21" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M20" s="46"/>
-      <c r="N20" s="46" t="s">
+      <c r="M21" s="76"/>
+      <c r="N21" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="O20" s="45"/>
-      <c r="P20" s="44" t="s">
+      <c r="O21" s="77"/>
+      <c r="P21" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="Q21" s="79">
         <v>6</v>
       </c>
-      <c r="R20" s="13" t="s">
+      <c r="R21" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="S20" s="13" t="s">
+      <c r="S21" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="T20" s="13" t="s">
+      <c r="T21" s="80" t="s">
         <v>180</v>
       </c>
-      <c r="U20" s="2" t="s">
+      <c r="U21" s="81" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21"/>
+      <c r="Z21"/>
+      <c r="AA21"/>
+      <c r="AB21"/>
+      <c r="AC21"/>
+      <c r="AD21"/>
+      <c r="AE21"/>
+      <c r="AF21"/>
+      <c r="AG21"/>
+      <c r="AH21"/>
+      <c r="AI21"/>
+      <c r="AJ21"/>
+      <c r="AK21"/>
+      <c r="AL21"/>
+      <c r="AM21"/>
+      <c r="AN21"/>
+      <c r="AO21"/>
+      <c r="AP21"/>
+      <c r="AQ21"/>
+      <c r="AR21"/>
+      <c r="AS21"/>
+      <c r="AT21"/>
+      <c r="AU21"/>
+      <c r="AV21"/>
+      <c r="AW21"/>
+      <c r="AX21"/>
+      <c r="AY21"/>
+      <c r="AZ21"/>
+    </row>
+    <row r="22" spans="1:52" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B22" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C22" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D22" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E22" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="F21" s="30" t="s">
+      <c r="F22" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="G21" s="36" t="s">
+      <c r="G22" s="71" t="s">
         <v>181</v>
       </c>
-      <c r="H21" s="37">
-        <v>15</v>
-      </c>
-      <c r="I21" s="37" t="s">
+      <c r="H22" s="74">
+        <v>16</v>
+      </c>
+      <c r="I22" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="50" t="s">
+      <c r="J22" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="K21" s="42" t="s">
+      <c r="K22" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="L21" s="43" t="s">
+      <c r="L22" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M21" s="46"/>
-      <c r="N21" s="46" t="s">
+      <c r="M22" s="76"/>
+      <c r="N22" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="O21" s="45"/>
-      <c r="P21" s="44" t="s">
+      <c r="O22" s="77"/>
+      <c r="P22" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="Q22" s="79">
         <v>6</v>
       </c>
-      <c r="R21" s="13" t="s">
+      <c r="R22" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="S21" s="13" t="s">
+      <c r="S22" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="T21" s="13" t="s">
+      <c r="T22" s="80" t="s">
         <v>183</v>
       </c>
-      <c r="U21" s="2" t="s">
+      <c r="U22" s="81" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+      <c r="Y22"/>
+      <c r="Z22"/>
+      <c r="AA22"/>
+      <c r="AB22"/>
+      <c r="AC22"/>
+      <c r="AD22"/>
+      <c r="AE22"/>
+      <c r="AF22"/>
+      <c r="AG22"/>
+      <c r="AH22"/>
+      <c r="AI22"/>
+      <c r="AJ22"/>
+      <c r="AK22"/>
+      <c r="AL22"/>
+      <c r="AM22"/>
+      <c r="AN22"/>
+      <c r="AO22"/>
+      <c r="AP22"/>
+      <c r="AQ22"/>
+      <c r="AR22"/>
+      <c r="AS22"/>
+      <c r="AT22"/>
+      <c r="AU22"/>
+      <c r="AV22"/>
+      <c r="AW22"/>
+      <c r="AX22"/>
+      <c r="AY22"/>
+      <c r="AZ22"/>
+    </row>
+    <row r="23" spans="1:52" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B23" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C23" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D23" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="E22" s="29" t="s">
+      <c r="E23" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="F22" s="30" t="s">
+      <c r="F23" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="G22" s="36" t="s">
+      <c r="G23" s="71" t="s">
         <v>184</v>
       </c>
-      <c r="H22" s="37">
-        <v>16</v>
-      </c>
-      <c r="I22" s="37" t="s">
+      <c r="H23" s="74">
+        <v>17</v>
+      </c>
+      <c r="I23" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="38" t="s">
+      <c r="J23" s="92" t="s">
         <v>187</v>
       </c>
-      <c r="K22" s="42" t="s">
+      <c r="K23" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="L22" s="43" t="s">
+      <c r="L23" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M22" s="46"/>
-      <c r="N22" s="46" t="s">
+      <c r="M23" s="76"/>
+      <c r="N23" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="O22" s="45"/>
-      <c r="P22" s="44" t="s">
+      <c r="O23" s="77"/>
+      <c r="P23" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="1">
+      <c r="Q23" s="79">
         <v>6</v>
       </c>
-      <c r="R22" s="13" t="s">
+      <c r="R23" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="S22" s="13" t="s">
+      <c r="S23" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="T22" s="13" t="s">
+      <c r="T23" s="80" t="s">
         <v>188</v>
       </c>
-      <c r="U22" s="2" t="s">
+      <c r="U23" s="81" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="V23"/>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="Y23"/>
+      <c r="Z23"/>
+      <c r="AA23"/>
+      <c r="AB23"/>
+      <c r="AC23"/>
+      <c r="AD23"/>
+      <c r="AE23"/>
+      <c r="AF23"/>
+      <c r="AG23"/>
+      <c r="AH23"/>
+      <c r="AI23"/>
+      <c r="AJ23"/>
+      <c r="AK23"/>
+      <c r="AL23"/>
+      <c r="AM23"/>
+      <c r="AN23"/>
+      <c r="AO23"/>
+      <c r="AP23"/>
+      <c r="AQ23"/>
+      <c r="AR23"/>
+      <c r="AS23"/>
+      <c r="AT23"/>
+      <c r="AU23"/>
+      <c r="AV23"/>
+      <c r="AW23"/>
+      <c r="AX23"/>
+      <c r="AY23"/>
+      <c r="AZ23"/>
+    </row>
+    <row r="24" spans="1:52" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B24" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C24" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D24" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="E23" s="29" t="s">
+      <c r="E24" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="F23" s="30" t="s">
+      <c r="F24" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="G23" s="36" t="s">
+      <c r="G24" s="71" t="s">
         <v>189</v>
       </c>
-      <c r="H23" s="37">
-        <v>17</v>
-      </c>
-      <c r="I23" s="37" t="s">
+      <c r="H24" s="74">
+        <v>18</v>
+      </c>
+      <c r="I24" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="50" t="s">
+      <c r="J24" s="83" t="s">
         <v>190</v>
       </c>
-      <c r="K23" s="42" t="s">
+      <c r="K24" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="L23" s="43" t="s">
+      <c r="L24" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46" t="s">
+      <c r="M24" s="76"/>
+      <c r="N24" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="O23" s="45"/>
-      <c r="P23" s="44" t="s">
+      <c r="O24" s="77"/>
+      <c r="P24" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="1">
+      <c r="Q24" s="79">
         <v>6</v>
       </c>
-      <c r="R23" s="13" t="s">
+      <c r="R24" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="S23" s="13" t="s">
+      <c r="S24" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="T23" s="13" t="s">
+      <c r="T24" s="80" t="s">
         <v>191</v>
       </c>
-      <c r="U23" s="2" t="s">
+      <c r="U24" s="81" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="Y24"/>
+      <c r="Z24"/>
+      <c r="AA24"/>
+      <c r="AB24"/>
+      <c r="AC24"/>
+      <c r="AD24"/>
+      <c r="AE24"/>
+      <c r="AF24"/>
+      <c r="AG24"/>
+      <c r="AH24"/>
+      <c r="AI24"/>
+      <c r="AJ24"/>
+      <c r="AK24"/>
+      <c r="AL24"/>
+      <c r="AM24"/>
+      <c r="AN24"/>
+      <c r="AO24"/>
+      <c r="AP24"/>
+      <c r="AQ24"/>
+      <c r="AR24"/>
+      <c r="AS24"/>
+      <c r="AT24"/>
+      <c r="AU24"/>
+      <c r="AV24"/>
+      <c r="AW24"/>
+      <c r="AX24"/>
+      <c r="AY24"/>
+      <c r="AZ24"/>
+    </row>
+    <row r="25" spans="1:52" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B25" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C25" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D25" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="E25" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="F24" s="30" t="s">
+      <c r="F25" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="G24" s="36" t="s">
+      <c r="G25" s="71" t="s">
         <v>193</v>
       </c>
-      <c r="H24" s="37">
-        <v>18</v>
-      </c>
-      <c r="I24" s="37" t="s">
+      <c r="H25" s="74">
+        <v>19</v>
+      </c>
+      <c r="I25" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="50" t="s">
+      <c r="J25" s="83" t="s">
         <v>195</v>
       </c>
-      <c r="K24" s="42" t="s">
+      <c r="K25" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="L24" s="43" t="s">
+      <c r="L25" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46" t="s">
+      <c r="M25" s="76"/>
+      <c r="N25" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="O24" s="45"/>
-      <c r="P24" s="44" t="s">
+      <c r="O25" s="77"/>
+      <c r="P25" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="Q24" s="1">
+      <c r="Q25" s="79">
         <v>6</v>
       </c>
-      <c r="R24" s="13" t="s">
+      <c r="R25" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="S24" s="13" t="s">
+      <c r="S25" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="T24" s="13" t="s">
+      <c r="T25" s="80" t="s">
         <v>196</v>
       </c>
-      <c r="U24" s="2" t="s">
+      <c r="U25" s="81" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25"/>
+      <c r="Z25"/>
+      <c r="AA25"/>
+      <c r="AB25"/>
+      <c r="AC25"/>
+      <c r="AD25"/>
+      <c r="AE25"/>
+      <c r="AF25"/>
+      <c r="AG25"/>
+      <c r="AH25"/>
+      <c r="AI25"/>
+      <c r="AJ25"/>
+      <c r="AK25"/>
+      <c r="AL25"/>
+      <c r="AM25"/>
+      <c r="AN25"/>
+      <c r="AO25"/>
+      <c r="AP25"/>
+      <c r="AQ25"/>
+      <c r="AR25"/>
+      <c r="AS25"/>
+      <c r="AT25"/>
+      <c r="AU25"/>
+      <c r="AV25"/>
+      <c r="AW25"/>
+      <c r="AX25"/>
+      <c r="AY25"/>
+      <c r="AZ25"/>
+    </row>
+    <row r="26" spans="1:52" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B26" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="G25" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="H25" s="37">
-        <v>19</v>
-      </c>
-      <c r="I25" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="K25" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="L25" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="M25" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="N25" s="46"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q25" s="1">
-        <v>6</v>
-      </c>
-      <c r="R25" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="S25" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="T25" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="U25" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="24" t="s">
         <v>92</v>
       </c>
       <c r="D26" s="25" t="s">
@@ -2903,15 +3370,46 @@
       <c r="U26" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="V26"/>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="Y26"/>
+      <c r="Z26"/>
+      <c r="AA26"/>
+      <c r="AB26"/>
+      <c r="AC26"/>
+      <c r="AD26"/>
+      <c r="AE26"/>
+      <c r="AF26"/>
+      <c r="AG26"/>
+      <c r="AH26"/>
+      <c r="AI26"/>
+      <c r="AJ26"/>
+      <c r="AK26"/>
+      <c r="AL26"/>
+      <c r="AM26"/>
+      <c r="AN26"/>
+      <c r="AO26"/>
+      <c r="AP26"/>
+      <c r="AQ26"/>
+      <c r="AR26"/>
+      <c r="AS26"/>
+      <c r="AT26"/>
+      <c r="AU26"/>
+      <c r="AV26"/>
+      <c r="AW26"/>
+      <c r="AX26"/>
+      <c r="AY26"/>
+      <c r="AZ26"/>
+    </row>
+    <row r="27" spans="1:52" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="24" t="s">
         <v>92</v>
       </c>
       <c r="D27" s="25" t="s">
@@ -2962,15 +3460,46 @@
       <c r="U27" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
+      <c r="V27"/>
+      <c r="W27"/>
+      <c r="X27"/>
+      <c r="Y27"/>
+      <c r="Z27"/>
+      <c r="AA27"/>
+      <c r="AB27"/>
+      <c r="AC27"/>
+      <c r="AD27"/>
+      <c r="AE27"/>
+      <c r="AF27"/>
+      <c r="AG27"/>
+      <c r="AH27"/>
+      <c r="AI27"/>
+      <c r="AJ27"/>
+      <c r="AK27"/>
+      <c r="AL27"/>
+      <c r="AM27"/>
+      <c r="AN27"/>
+      <c r="AO27"/>
+      <c r="AP27"/>
+      <c r="AQ27"/>
+      <c r="AR27"/>
+      <c r="AS27"/>
+      <c r="AT27"/>
+      <c r="AU27"/>
+      <c r="AV27"/>
+      <c r="AW27"/>
+      <c r="AX27"/>
+      <c r="AY27"/>
+      <c r="AZ27"/>
+    </row>
+    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="24" t="s">
         <v>92</v>
       </c>
       <c r="D28" s="25" t="s">
@@ -2996,14 +3525,14 @@
       <c r="T28" s="13"/>
       <c r="U28" s="2"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
+    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="24" t="s">
         <v>92</v>
       </c>
       <c r="D29" s="25" t="s">
@@ -3029,7 +3558,7 @@
       <c r="T29" s="13"/>
       <c r="U29" s="2"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>67</v>
       </c>
@@ -3062,7 +3591,7 @@
       <c r="T30" s="13"/>
       <c r="U30" s="2"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>67</v>
       </c>
@@ -3121,233 +3650,235 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
+    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A32" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="25" t="s">
+      <c r="D32" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="E32" s="29" t="s">
+      <c r="E32" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="57"/>
+      <c r="G32" s="55" t="s">
+        <v>200</v>
+      </c>
+      <c r="H32" s="58">
+        <v>23</v>
+      </c>
+      <c r="I32" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="J32" s="59" t="s">
+        <v>201</v>
+      </c>
+      <c r="K32" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="L32" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="M32" s="61"/>
+      <c r="N32" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="O32" s="62"/>
+      <c r="P32" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q32" s="64">
+        <v>6</v>
+      </c>
+      <c r="R32" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="S32" s="65" t="s">
+        <v>140</v>
+      </c>
+      <c r="T32" s="65" t="s">
+        <v>202</v>
+      </c>
+      <c r="U32" s="66" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="70" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="71" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="F32" s="30"/>
-      <c r="G32" s="50" t="s">
+      <c r="F33" s="73"/>
+      <c r="G33" s="83" t="s">
         <v>146</v>
       </c>
-      <c r="H32" s="37">
-        <v>23</v>
-      </c>
-      <c r="I32" s="37" t="s">
+      <c r="H33" s="74">
+        <v>24</v>
+      </c>
+      <c r="I33" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J32" s="38" t="s">
+      <c r="J33" s="92" t="s">
         <v>147</v>
       </c>
-      <c r="K32" s="42" t="s">
+      <c r="K33" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="L32" s="43" t="s">
+      <c r="L33" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M32" s="46"/>
-      <c r="N32" s="46" t="s">
+      <c r="M33" s="76"/>
+      <c r="N33" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="O32" s="45"/>
-      <c r="P32" s="44" t="s">
+      <c r="O33" s="77"/>
+      <c r="P33" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q32" s="1">
+      <c r="Q33" s="79">
         <v>6</v>
       </c>
-      <c r="R32" s="13" t="s">
+      <c r="R33" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="S32" s="13" t="s">
+      <c r="S33" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="T32" s="13" t="s">
+      <c r="T33" s="80" t="s">
         <v>148</v>
       </c>
-      <c r="U32" s="2" t="s">
+      <c r="U33" s="81" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B34" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C34" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="25" t="s">
+      <c r="D34" s="71" t="s">
         <v>116</v>
       </c>
-      <c r="E33" s="29"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="36" t="s">
+      <c r="E34" s="72"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="71" t="s">
         <v>149</v>
       </c>
-      <c r="H33" s="37">
-        <v>24</v>
-      </c>
-      <c r="I33" s="37" t="s">
+      <c r="H34" s="74">
+        <v>25</v>
+      </c>
+      <c r="I34" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J33" s="38" t="s">
+      <c r="J34" s="92" t="s">
         <v>150</v>
       </c>
-      <c r="K33" s="42" t="s">
+      <c r="K34" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="L33" s="43" t="s">
+      <c r="L34" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M33" s="46"/>
-      <c r="N33" s="46" t="s">
+      <c r="M34" s="76"/>
+      <c r="N34" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="O33" s="45"/>
-      <c r="P33" s="44" t="s">
+      <c r="O34" s="77"/>
+      <c r="P34" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q33" s="1">
+      <c r="Q34" s="79">
         <v>6</v>
       </c>
-      <c r="R33" s="13" t="s">
+      <c r="R34" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="S33" s="13" t="s">
+      <c r="S34" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="T33" s="13" t="s">
+      <c r="T34" s="80" t="s">
         <v>151</v>
       </c>
-      <c r="U33" s="2" t="s">
+      <c r="U34" s="81" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B35" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C35" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="D34" s="25" t="s">
+      <c r="D35" s="71" t="s">
         <v>116</v>
       </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="36" t="s">
+      <c r="E35" s="72"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="71" t="s">
         <v>212</v>
       </c>
-      <c r="H34" s="37">
-        <v>25</v>
-      </c>
-      <c r="I34" s="37" t="s">
+      <c r="H35" s="74">
+        <v>26</v>
+      </c>
+      <c r="I35" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J34" s="38" t="s">
+      <c r="J35" s="92" t="s">
         <v>213</v>
       </c>
-      <c r="K34" s="42" t="s">
+      <c r="K35" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="L34" s="43" t="s">
+      <c r="L35" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M34" s="46"/>
-      <c r="N34" s="46" t="s">
+      <c r="M35" s="76"/>
+      <c r="N35" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="O34" s="45"/>
-      <c r="P34" s="44" t="s">
+      <c r="O35" s="77"/>
+      <c r="P35" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q34" s="1">
+      <c r="Q35" s="79">
         <v>6</v>
       </c>
-      <c r="R34" s="13" t="s">
+      <c r="R35" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="S34" s="13" t="s">
+      <c r="S35" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="T34" s="13" t="s">
+      <c r="T35" s="80" t="s">
         <v>152</v>
       </c>
-      <c r="U34" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="36" t="s">
-        <v>200</v>
-      </c>
-      <c r="H35" s="37">
-        <v>26</v>
-      </c>
-      <c r="I35" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="J35" s="38" t="s">
-        <v>201</v>
-      </c>
-      <c r="K35" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="L35" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="M35" s="46"/>
-      <c r="N35" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="O35" s="45"/>
-      <c r="P35" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q35" s="1">
-        <v>6</v>
-      </c>
-      <c r="R35" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="S35" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="T35" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="U35" s="2" t="s">
+      <c r="U35" s="81" t="s">
         <v>142</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambio nombre de recursos
Cambio nombre de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion09/ESCALETAFINAL CN_09_09_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion09/ESCALETAFINAL CN_09_09_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado09\guion09\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="219">
   <si>
     <t>Asignatura</t>
   </si>
@@ -399,9 +399,6 @@
     <t>RM_01_02_CO</t>
   </si>
   <si>
-    <t>Interactivo que facilita trabajar la solubilidad de una sal en agua</t>
-  </si>
-  <si>
     <t>3º ESO</t>
   </si>
   <si>
@@ -666,9 +663,6 @@
     <t>Secuencia de imágenes que permite explicar las caracteristicas de las disoluciones y el proceso de disolución</t>
   </si>
   <si>
-    <t>Animación que permite explicar la ósmosis y la presión osmótica</t>
-  </si>
-  <si>
     <t xml:space="preserve">Competencias: preparación de un producto de cuidado personal </t>
   </si>
   <si>
@@ -679,6 +673,21 @@
   </si>
   <si>
     <t>Actividad que permite ejercitar los cálculos de concentración de disoluciones en porcentaje en masa-volumen</t>
+  </si>
+  <si>
+    <t>La ósmosis y la presión osmótica</t>
+  </si>
+  <si>
+    <t>Animación que permite explicar el fenómeno de la ósmosis y la presión osmótica</t>
+  </si>
+  <si>
+    <t>Los sistemas homogéneos o disoluciones</t>
+  </si>
+  <si>
+    <t>La solubilidad de una sal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactivo que permite mostrar la influencia de la temperatura en la solubilidad de una sal </t>
   </si>
 </sst>
 </file>
@@ -1204,6 +1213,9 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1227,9 +1239,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1513,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,94 +1551,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="84" t="s">
+      <c r="C1" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="84" t="s">
+      <c r="D1" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="84" t="s">
+      <c r="E1" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="84" t="s">
+      <c r="F1" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="84" t="s">
+      <c r="G1" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="84" t="s">
+      <c r="H1" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="84" t="s">
+      <c r="I1" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="84" t="s">
+      <c r="J1" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="88" t="s">
+      <c r="K1" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="86" t="s">
+      <c r="L1" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="90" t="s">
+      <c r="M1" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="91"/>
-      <c r="O1" s="84" t="s">
+      <c r="N1" s="92"/>
+      <c r="O1" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="84" t="s">
+      <c r="P1" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="84" t="s">
+      <c r="Q1" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="84" t="s">
+      <c r="R1" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="84" t="s">
+      <c r="S1" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="84" t="s">
+      <c r="T1" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="84" t="s">
+      <c r="U1" s="85" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:52" s="12" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="85"/>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="87"/>
+      <c r="A2" s="86"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="88"/>
       <c r="M2" s="51" t="s">
         <v>87</v>
       </c>
       <c r="N2" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="85"/>
-      <c r="U2" s="85"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="86"/>
+      <c r="S2" s="86"/>
+      <c r="T2" s="86"/>
+      <c r="U2" s="86"/>
       <c r="V2"/>
       <c r="W2"/>
       <c r="X2"/>
@@ -1685,7 +1694,7 @@
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="36" t="s">
-        <v>92</v>
+        <v>216</v>
       </c>
       <c r="H4" s="37">
         <v>1</v>
@@ -1694,7 +1703,7 @@
         <v>19</v>
       </c>
       <c r="J4" s="38" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K4" s="42" t="s">
         <v>69</v>
@@ -1847,7 +1856,7 @@
       </c>
       <c r="F8" s="30"/>
       <c r="G8" s="36" t="s">
-        <v>98</v>
+        <v>217</v>
       </c>
       <c r="H8" s="37">
         <v>2</v>
@@ -1856,7 +1865,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="38" t="s">
-        <v>122</v>
+        <v>218</v>
       </c>
       <c r="K8" s="42" t="s">
         <v>70</v>
@@ -1871,19 +1880,19 @@
         <v>19</v>
       </c>
       <c r="Q8" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="R8" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="R8" s="13" t="s">
+      <c r="S8" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="S8" s="13" t="s">
+      <c r="T8" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="T8" s="13" t="s">
+      <c r="U8" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
@@ -1904,7 +1913,7 @@
       </c>
       <c r="F9" s="30"/>
       <c r="G9" s="36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H9" s="37">
         <v>3</v>
@@ -1913,7 +1922,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K9" s="42" t="s">
         <v>69</v>
@@ -1936,13 +1945,13 @@
         <v>118</v>
       </c>
       <c r="S9" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T9" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.25">
@@ -1963,7 +1972,7 @@
       </c>
       <c r="F10" s="30"/>
       <c r="G10" s="36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H10" s="37">
         <v>4</v>
@@ -1972,7 +1981,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K10" s="42" t="s">
         <v>70</v>
@@ -1987,19 +1996,19 @@
         <v>20</v>
       </c>
       <c r="Q10" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="R10" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="R10" s="13" t="s">
+      <c r="S10" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="S10" s="13" t="s">
-        <v>125</v>
-      </c>
       <c r="T10" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.25">
@@ -2020,7 +2029,7 @@
       </c>
       <c r="F11" s="30"/>
       <c r="G11" s="50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H11" s="37">
         <v>5</v>
@@ -2029,7 +2038,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K11" s="42" t="s">
         <v>69</v>
@@ -2052,13 +2061,13 @@
         <v>118</v>
       </c>
       <c r="S11" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T11" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.25">
@@ -2079,7 +2088,7 @@
       </c>
       <c r="F12" s="28"/>
       <c r="G12" s="36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H12" s="37">
         <v>6</v>
@@ -2088,7 +2097,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K12" s="42" t="s">
         <v>69</v>
@@ -2111,13 +2120,13 @@
         <v>118</v>
       </c>
       <c r="S12" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="T12" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="T12" s="13" t="s">
+      <c r="U12" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:52" s="67" customFormat="1" x14ac:dyDescent="0.25">
@@ -2138,7 +2147,7 @@
       </c>
       <c r="F13" s="57"/>
       <c r="G13" s="55" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H13" s="58">
         <v>7</v>
@@ -2147,7 +2156,7 @@
         <v>19</v>
       </c>
       <c r="J13" s="59" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K13" s="56" t="s">
         <v>69</v>
@@ -2167,16 +2176,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="S13" s="65" t="s">
         <v>131</v>
       </c>
-      <c r="S13" s="65" t="s">
+      <c r="T13" s="65" t="s">
         <v>132</v>
       </c>
-      <c r="T13" s="65" t="s">
+      <c r="U13" s="66" t="s">
         <v>133</v>
-      </c>
-      <c r="U13" s="66" t="s">
-        <v>134</v>
       </c>
       <c r="V13"/>
       <c r="W13"/>
@@ -2230,7 +2239,7 @@
         <v>103</v>
       </c>
       <c r="G14" s="71" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H14" s="74">
         <v>8</v>
@@ -2239,7 +2248,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="83" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K14" s="72" t="s">
         <v>69</v>
@@ -2262,13 +2271,13 @@
         <v>118</v>
       </c>
       <c r="S14" s="80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T14" s="80" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="U14" s="81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V14"/>
       <c r="W14"/>
@@ -2322,7 +2331,7 @@
         <v>104</v>
       </c>
       <c r="G15" s="71" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H15" s="74">
         <v>9</v>
@@ -2331,7 +2340,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="83" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K15" s="72" t="s">
         <v>69</v>
@@ -2354,13 +2363,13 @@
         <v>118</v>
       </c>
       <c r="S15" s="80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T15" s="80" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="U15" s="81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V15"/>
       <c r="W15"/>
@@ -2411,10 +2420,10 @@
         <v>102</v>
       </c>
       <c r="F16" s="73" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G16" s="71" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H16" s="74">
         <v>10</v>
@@ -2423,7 +2432,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="83" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K16" s="72" t="s">
         <v>69</v>
@@ -2446,13 +2455,13 @@
         <v>118</v>
       </c>
       <c r="S16" s="80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T16" s="80" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="U16" s="81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V16"/>
       <c r="W16" t="s">
@@ -2508,7 +2517,7 @@
         <v>105</v>
       </c>
       <c r="G17" s="71" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H17" s="74">
         <v>11</v>
@@ -2517,7 +2526,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="83" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K17" s="72" t="s">
         <v>69</v>
@@ -2540,13 +2549,13 @@
         <v>118</v>
       </c>
       <c r="S17" s="80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T17" s="80" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U17" s="81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V17"/>
       <c r="W17"/>
@@ -2600,7 +2609,7 @@
         <v>105</v>
       </c>
       <c r="G18" s="71" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H18" s="74">
         <v>12</v>
@@ -2609,7 +2618,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="83" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K18" s="72" t="s">
         <v>69</v>
@@ -2632,13 +2641,13 @@
         <v>118</v>
       </c>
       <c r="S18" s="80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T18" s="80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="U18" s="81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V18"/>
       <c r="W18"/>
@@ -2690,7 +2699,7 @@
       </c>
       <c r="F19" s="57"/>
       <c r="G19" s="55" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H19" s="58">
         <v>13</v>
@@ -2699,7 +2708,7 @@
         <v>19</v>
       </c>
       <c r="J19" s="59" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K19" s="56" t="s">
         <v>69</v>
@@ -2719,16 +2728,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="S19" s="65" t="s">
         <v>131</v>
       </c>
-      <c r="S19" s="65" t="s">
-        <v>132</v>
-      </c>
       <c r="T19" s="65" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="U19" s="66" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="V19"/>
       <c r="W19"/>
@@ -2780,7 +2789,7 @@
       </c>
       <c r="F20" s="73"/>
       <c r="G20" s="71" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H20" s="74">
         <v>14</v>
@@ -2788,8 +2797,8 @@
       <c r="I20" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="92" t="s">
-        <v>167</v>
+      <c r="J20" s="84" t="s">
+        <v>166</v>
       </c>
       <c r="K20" s="72" t="s">
         <v>70</v>
@@ -2800,25 +2809,25 @@
       <c r="M20" s="76"/>
       <c r="N20" s="76"/>
       <c r="O20" s="77" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P20" s="78" t="s">
         <v>19</v>
       </c>
       <c r="Q20" s="79" t="s">
+        <v>122</v>
+      </c>
+      <c r="R20" s="80" t="s">
         <v>123</v>
       </c>
-      <c r="R20" s="80" t="s">
+      <c r="S20" s="80" t="s">
         <v>124</v>
       </c>
-      <c r="S20" s="80" t="s">
-        <v>125</v>
-      </c>
       <c r="T20" s="80" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="U20" s="81" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="V20"/>
       <c r="W20"/>
@@ -2872,7 +2881,7 @@
         <v>107</v>
       </c>
       <c r="G21" s="71" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H21" s="74">
         <v>15</v>
@@ -2881,7 +2890,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="83" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K21" s="72" t="s">
         <v>69</v>
@@ -2904,13 +2913,13 @@
         <v>118</v>
       </c>
       <c r="S21" s="80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T21" s="80" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="U21" s="81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V21"/>
       <c r="W21"/>
@@ -2964,7 +2973,7 @@
         <v>108</v>
       </c>
       <c r="G22" s="71" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H22" s="74">
         <v>16</v>
@@ -2973,7 +2982,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="83" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K22" s="72" t="s">
         <v>69</v>
@@ -2996,13 +3005,13 @@
         <v>118</v>
       </c>
       <c r="S22" s="80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T22" s="80" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="U22" s="81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V22"/>
       <c r="W22"/>
@@ -3056,7 +3065,7 @@
         <v>109</v>
       </c>
       <c r="G23" s="71" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H23" s="74">
         <v>17</v>
@@ -3064,8 +3073,8 @@
       <c r="I23" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="92" t="s">
-        <v>187</v>
+      <c r="J23" s="84" t="s">
+        <v>186</v>
       </c>
       <c r="K23" s="72" t="s">
         <v>69</v>
@@ -3088,13 +3097,13 @@
         <v>118</v>
       </c>
       <c r="S23" s="80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T23" s="80" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U23" s="81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V23"/>
       <c r="W23"/>
@@ -3148,7 +3157,7 @@
         <v>109</v>
       </c>
       <c r="G24" s="71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H24" s="74">
         <v>18</v>
@@ -3157,7 +3166,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="83" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K24" s="72" t="s">
         <v>69</v>
@@ -3180,13 +3189,13 @@
         <v>118</v>
       </c>
       <c r="S24" s="80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T24" s="80" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="U24" s="81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V24"/>
       <c r="W24"/>
@@ -3240,7 +3249,7 @@
         <v>109</v>
       </c>
       <c r="G25" s="71" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H25" s="74">
         <v>19</v>
@@ -3249,7 +3258,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="83" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K25" s="72" t="s">
         <v>69</v>
@@ -3272,13 +3281,13 @@
         <v>118</v>
       </c>
       <c r="S25" s="80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T25" s="80" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="U25" s="81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V25"/>
       <c r="W25"/>
@@ -3330,7 +3339,7 @@
       </c>
       <c r="F26" s="30"/>
       <c r="G26" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H26" s="37">
         <v>20</v>
@@ -3339,7 +3348,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K26" s="42" t="s">
         <v>69</v>
@@ -3362,13 +3371,13 @@
         <v>118</v>
       </c>
       <c r="S26" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T26" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="U26" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V26"/>
       <c r="W26"/>
@@ -3420,7 +3429,7 @@
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H27" s="37">
         <v>21</v>
@@ -3429,7 +3438,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K27" s="42" t="s">
         <v>69</v>
@@ -3452,13 +3461,13 @@
         <v>118</v>
       </c>
       <c r="S27" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T27" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="U27" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V27"/>
       <c r="W27"/>
@@ -3609,7 +3618,7 @@
       </c>
       <c r="F31" s="30"/>
       <c r="G31" s="36" t="s">
-        <v>115</v>
+        <v>214</v>
       </c>
       <c r="H31" s="37">
         <v>22</v>
@@ -3618,7 +3627,7 @@
         <v>19</v>
       </c>
       <c r="J31" s="38" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="K31" s="42" t="s">
         <v>69</v>
@@ -3638,16 +3647,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="S31" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="S31" s="13" t="s">
-        <v>132</v>
-      </c>
       <c r="T31" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="U31" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.25">
@@ -3668,7 +3677,7 @@
       </c>
       <c r="F32" s="57"/>
       <c r="G32" s="55" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H32" s="58">
         <v>23</v>
@@ -3677,7 +3686,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="59" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K32" s="56" t="s">
         <v>69</v>
@@ -3700,13 +3709,13 @@
         <v>118</v>
       </c>
       <c r="S32" s="65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T32" s="65" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U32" s="66" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -3727,7 +3736,7 @@
       </c>
       <c r="F33" s="73"/>
       <c r="G33" s="83" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H33" s="74">
         <v>24</v>
@@ -3735,8 +3744,8 @@
       <c r="I33" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J33" s="92" t="s">
-        <v>147</v>
+      <c r="J33" s="84" t="s">
+        <v>146</v>
       </c>
       <c r="K33" s="72" t="s">
         <v>69</v>
@@ -3759,13 +3768,13 @@
         <v>118</v>
       </c>
       <c r="S33" s="80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T33" s="80" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="U33" s="81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -3784,7 +3793,7 @@
       <c r="E34" s="72"/>
       <c r="F34" s="73"/>
       <c r="G34" s="71" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H34" s="74">
         <v>25</v>
@@ -3792,8 +3801,8 @@
       <c r="I34" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J34" s="92" t="s">
-        <v>150</v>
+      <c r="J34" s="84" t="s">
+        <v>149</v>
       </c>
       <c r="K34" s="72" t="s">
         <v>69</v>
@@ -3816,13 +3825,13 @@
         <v>118</v>
       </c>
       <c r="S34" s="80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T34" s="80" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="U34" s="81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
@@ -3841,7 +3850,7 @@
       <c r="E35" s="72"/>
       <c r="F35" s="73"/>
       <c r="G35" s="71" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H35" s="74">
         <v>26</v>
@@ -3849,8 +3858,8 @@
       <c r="I35" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J35" s="92" t="s">
-        <v>213</v>
+      <c r="J35" s="84" t="s">
+        <v>211</v>
       </c>
       <c r="K35" s="72" t="s">
         <v>69</v>
@@ -3873,13 +3882,13 @@
         <v>118</v>
       </c>
       <c r="S35" s="80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T35" s="80" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="U35" s="81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
@@ -3893,12 +3902,12 @@
         <v>92</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E36" s="29"/>
       <c r="F36" s="30"/>
       <c r="G36" s="36" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H36" s="37">
         <v>27</v>
@@ -3907,7 +3916,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K36" s="42" t="s">
         <v>69</v>
@@ -3938,12 +3947,12 @@
         <v>92</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E37" s="29"/>
       <c r="F37" s="30"/>
       <c r="G37" s="36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H37" s="37">
         <v>28</v>
@@ -3952,7 +3961,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K37" s="42" t="s">
         <v>69</v>
@@ -3975,13 +3984,13 @@
         <v>118</v>
       </c>
       <c r="S37" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T37" s="13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U37" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -3998,7 +4007,7 @@
       <c r="E38" s="29"/>
       <c r="F38" s="30"/>
       <c r="G38" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H38" s="37">
         <v>29</v>
@@ -4007,7 +4016,7 @@
         <v>20</v>
       </c>
       <c r="J38" s="38" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K38" s="42" t="s">
         <v>69</v>
@@ -4030,13 +4039,13 @@
         <v>118</v>
       </c>
       <c r="S38" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T38" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U38" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
@@ -5467,6 +5476,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="U1:U2"/>
@@ -5482,11 +5496,6 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>